<commit_message>
Added stock to dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506A9181-DD51-494A-AA97-87B41FFD476F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E45D39-0AF5-5245-AF1F-B1A92E5F8215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="16" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
     <sheet name="Ledger" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -35,24 +35,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={B734B965-24A6-479B-9B64-AC439E271E9A}</author>
-  </authors>
-  <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{B734B965-24A6-479B-9B64-AC439E271E9A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Buy, Sell, DRIP</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -255,7 +237,7 @@
     <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,9 +267,16 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="21"/>
+      <sz val="25"/>
       <color theme="0"/>
       <name val="Britannic Bold"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -322,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -335,16 +324,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -385,9 +377,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Mynda Treacy" id="{11AAC28B-932D-4D2E-A823-16C458804BEB}" userId="Mynda Treacy" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,6 +536,158 @@
     <v>1</v>
   </rv>
   <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=aa5c2w&amp;q=XASX%3aCAT&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="3">
+    <v>5</v>
+    <v>CATAPULT GROUP INTERNATIONAL LTD (XASX:CAT)</v>
+    <v>2</v>
+    <v>6</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-AU</v>
+    <v>aa5c2w</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>1.5349999999999999</v>
+    <v>0.70499999999999996</v>
+    <v>2.4112</v>
+    <v>-2.5000000000000001E-2</v>
+    <v>-3.4247E-2</v>
+    <v>AUD</v>
+    <v>Catapult Group International Limited is an Australia-based company engaged in the development and supply of technologies that improve the performance of athletes and sports teams. The Company operates at the intersection of sports science and analytics. The Company operates through three segments: Performance &amp; Health, Tactics &amp; Coaching and Media &amp; Other. Its Performance &amp; Health segment is engaged in the design, development and supply of wearable technology and athlete monitoring software solutions to sports teams, athletes and the prosumer market. Its Tactics &amp; Coaching segment is engaged in the design, development and supply of video analysis, editing, and publishing software solutions to sports teams. Its Media &amp; Other segment provides media licensing, athlete management and professional services to customers. The Company operates through its subsidiary, Catapult Sports Inc.</v>
+    <v>Australian Securities Exchange</v>
+    <v>XASX</v>
+    <v>XASX</v>
+    <v>75 - 83 High Street, PRAHAN, VICTORIA, 3181 AU</v>
+    <v>0.73</v>
+    <v>Electronic Equipment &amp; Parts</v>
+    <v>Stock</v>
+    <v>44951.333333333336</v>
+    <v>3</v>
+    <v>0.70499999999999996</v>
+    <v>178162300</v>
+    <v>CATAPULT GROUP INTERNATIONAL LTD</v>
+    <v>CATAPULT GROUP INTERNATIONAL LTD</v>
+    <v>0.73</v>
+    <v>28.45</v>
+    <v>0.73</v>
+    <v>0.70499999999999996</v>
+    <v>244057900</v>
+    <v>CAT</v>
+    <v>CATAPULT GROUP INTERNATIONAL LTD (XASX:CAT)</v>
+    <v>95020</v>
+    <v>62270</v>
+    <v>2013</v>
+  </rv>
+  <rv s="2">
+    <v>4</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=aa5cec&amp;q=XASX%3aCBA&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>COMMONWEALTH BANK OF AUSTRALIA (XASX:CBA)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-AU</v>
+    <v>aa5cec</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>109.2</v>
+    <v>86.98</v>
+    <v>1.0513999999999999</v>
+    <v>0.78</v>
+    <v>7.2189999999999997E-3</v>
+    <v>AUD</v>
+    <v>Commonwealth Bank of Australia is an Australia-based provider of financial services in Australia. The Company provides retail and commercial banking services predominantly in Australia and in New Zealand through its subsidiary, ASB. It serves approximately 15 million customers. It operates through two segments. The retail management segment has sub-segments covering housing loan, credit cards, personal loans and personal overdrafts. It also covers most non-retail lending where the aggregate credit exposure to a group of related borrowers is less than one million dollars. Auto-decisioning is used to approve credit applications for eligible borrowers in this segment. The risk-rating segment comprises non-retail exposures, including bank and sovereign exposures. Each exposure is assigned an internal Credit Risk-Rating (CRR) based on Probability of Default (PD) and Loss Given Default (LGD). Either a PD Rating Tool or expert judgment is used to determine the PD for customers in this segment</v>
+    <v>49245</v>
+    <v>Australian Securities Exchange</v>
+    <v>XASX</v>
+    <v>XASX</v>
+    <v>Ground Floor, Tower 1, 201 Sussex Street, SYDNEY, NEW SOUTH WALES, 2000 AU</v>
+    <v>109.2</v>
+    <v>Banking Services</v>
+    <v>Stock</v>
+    <v>44951.333333333336</v>
+    <v>6</v>
+    <v>107.79</v>
+    <v>182433200000</v>
+    <v>COMMONWEALTH BANK OF AUSTRALIA</v>
+    <v>COMMONWEALTH BANK OF AUSTRALIA</v>
+    <v>108.01</v>
+    <v>17.28</v>
+    <v>108.05</v>
+    <v>108.83</v>
+    <v>1688414000</v>
+    <v>CBA</v>
+    <v>COMMONWEALTH BANK OF AUSTRALIA (XASX:CBA)</v>
+    <v>1620732</v>
+    <v>2025450</v>
+    <v>1991</v>
+  </rv>
+  <rv s="2">
+    <v>7</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=aa658m&amp;q=XASX%3aEOS&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED (XASX:EOS)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-AU</v>
+    <v>aa658m</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>3.38</v>
+    <v>0.43</v>
+    <v>2.3931</v>
+    <v>-0.02</v>
+    <v>-2.8986000000000001E-2</v>
+    <v>AUD</v>
+    <v>Electro Optic Systems Holdings Limited is an Australia-based technology company. The Company’s segments include Defense Systems, Space Systems and Communications Systems. The Company’s Defense Systems develops, manufactures and markets fire control, surveillance and weapon systems to approved military customers. The Company’s Space Systems specializes in the design, manufacture, delivery and operation of sensors and systems for space domain awareness (SDA) and space control. The Company’s Communications Systems develops and provides global satellite communications products, systems and services. The Communications Systems specializes in optical, microwave and on-the-move radio and satellite systems that deliver telecommunications anywhere in the world. The Company's products incorporate electro-optic applications based on its technologies in software, laser, electronics, optronics, gimbals, telescopes and beam directors and mechanisms.</v>
+    <v>218</v>
+    <v>Australian Securities Exchange</v>
+    <v>XASX</v>
+    <v>XASX</v>
+    <v>18 Wormald Street, Symonston, AUSTRALIAN CAPITAL TERRITORY, 2609 AU</v>
+    <v>0.71</v>
+    <v>Aerospace &amp; Defense</v>
+    <v>Stock</v>
+    <v>44951.333333333336</v>
+    <v>9</v>
+    <v>0.65</v>
+    <v>118152800</v>
+    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED</v>
+    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED</v>
+    <v>0.67500000000000004</v>
+    <v>28.53</v>
+    <v>0.69</v>
+    <v>0.67</v>
+    <v>171236000</v>
+    <v>EOS</v>
+    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED (XASX:EOS)</v>
+    <v>353942</v>
+    <v>700850</v>
+    <v>2000</v>
+  </rv>
+  <rv s="2">
+    <v>10</v>
+  </rv>
+  <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa81zr&amp;q=XASX%3aNAB&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
@@ -577,7 +719,7 @@
     <v>Banking Services</v>
     <v>Stock</v>
     <v>44951.333333333336</v>
-    <v>3</v>
+    <v>12</v>
     <v>31.25</v>
     <v>98662430000</v>
     <v>NATIONAL AUSTRALIA BANK LIMITED</v>
@@ -594,7 +736,58 @@
     <v>1893</v>
   </rv>
   <rv s="2">
+    <v>13</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=aa86z2&amp;q=XASX%3aNEA&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="4">
+    <v>7</v>
+    <v>NEARMAP LTD (XASX:NEA)</v>
+    <v>2</v>
+    <v>8</v>
+    <v>Finance</v>
     <v>4</v>
+    <v>en-AU</v>
+    <v>aa86z2</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>2.79</v>
+    <v>1.37</v>
+    <v>1.7012</v>
+    <v>0.01</v>
+    <v>6.515E-3</v>
+    <v>AUD</v>
+    <v>Nearmap Ltd is an Australia-based location intelligence company that provides cloud-based geospatial information services. The Company's is engaged in providing online aerial photomaps to business customers via subscription through its subsidiaries, Nearmap Australia Pty Ltd and Nearmap US, Inc. The Company uses its camera systems and processing software to conduct aerial surveys that captures wide-scale urban areas in Australia, New Zealand, the United States of America, and Canada multiple times each year, making fresh content instantly available in the cloud via Web application or application programming interface (API) integration. The Company's products include Vertical Imagery, Oblique Imagery, 3D Imagery and Data, Nearmap AI, and Nearmap on OpenSolar. The Company serves various industries, including Government, construction, telecommunication, transportation, insurance, property, roofing, and solar.</v>
+    <v>400</v>
+    <v>Australian Securities Exchange</v>
+    <v>XASX</v>
+    <v>XASX</v>
+    <v>Tower 1, International Towers Sydney L 4, 100 Barangaroo Ave, SYDNEY, NEW SOUTH WALES, 2000 AU</v>
+    <v>1.57</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>44552.02238425926</v>
+    <v>15</v>
+    <v>1.54</v>
+    <v>768177100</v>
+    <v>NEARMAP LTD</v>
+    <v>NEARMAP LTD</v>
+    <v>1.57</v>
+    <v>34.51</v>
+    <v>1.5349999999999999</v>
+    <v>1.5449999999999999</v>
+    <v>498816300</v>
+    <v>NEA</v>
+    <v>NEARMAP LTD (XASX:NEA)</v>
+    <v>509998</v>
+    <v>1998</v>
+  </rv>
+  <rv s="2">
+    <v>16</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa759c&amp;q=XASX%3aIVC&amp;form=skydnc</v>
@@ -628,7 +821,7 @@
     <v>Personal &amp; Household Products &amp; Services</v>
     <v>Stock</v>
     <v>44951.333333333336</v>
-    <v>6</v>
+    <v>18</v>
     <v>11.35</v>
     <v>1637971000</v>
     <v>INVOCARE LIMITED</v>
@@ -645,17 +838,17 @@
     <v>2001</v>
   </rv>
   <rv s="2">
-    <v>7</v>
+    <v>19</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa5rc7&amp;q=XASX%3aCWN&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="4">
+    <v>7</v>
     <v>CROWN RESORTS LIMITED (XASX:CWN)</v>
     <v>2</v>
-    <v>6</v>
+    <v>8</v>
     <v>Finance</v>
     <v>4</v>
     <v>en-AU</v>
@@ -680,7 +873,7 @@
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
     <v>44552.022349537037</v>
-    <v>9</v>
+    <v>21</v>
     <v>11.39</v>
     <v>7557086000</v>
     <v>CROWN RESORTS LIMITED</v>
@@ -696,7 +889,7 @@
     <v>2007</v>
   </rv>
   <rv s="2">
-    <v>10</v>
+    <v>22</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa8rvh&amp;q=XASX%3aQAN&amp;form=skydnc</v>
@@ -730,7 +923,7 @@
     <v>Passenger Transportation Services</v>
     <v>Stock</v>
     <v>44951.333333333336</v>
-    <v>12</v>
+    <v>24</v>
     <v>6.41</v>
     <v>11646050000</v>
     <v>QANTAS AIRWAYS LIMITED</v>
@@ -745,209 +938,6 @@
     <v>5260501</v>
     <v>5943190</v>
     <v>1934</v>
-  </rv>
-  <rv s="2">
-    <v>13</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=aa5cec&amp;q=XASX%3aCBA&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="1">
-    <v>0</v>
-    <v>COMMONWEALTH BANK OF AUSTRALIA (XASX:CBA)</v>
-    <v>2</v>
-    <v>3</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-AU</v>
-    <v>aa5cec</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>109.2</v>
-    <v>86.98</v>
-    <v>1.0513999999999999</v>
-    <v>0.78</v>
-    <v>7.2189999999999997E-3</v>
-    <v>AUD</v>
-    <v>Commonwealth Bank of Australia is an Australia-based provider of financial services in Australia. The Company provides retail and commercial banking services predominantly in Australia and in New Zealand through its subsidiary, ASB. It serves approximately 15 million customers. It operates through two segments. The retail management segment has sub-segments covering housing loan, credit cards, personal loans and personal overdrafts. It also covers most non-retail lending where the aggregate credit exposure to a group of related borrowers is less than one million dollars. Auto-decisioning is used to approve credit applications for eligible borrowers in this segment. The risk-rating segment comprises non-retail exposures, including bank and sovereign exposures. Each exposure is assigned an internal Credit Risk-Rating (CRR) based on Probability of Default (PD) and Loss Given Default (LGD). Either a PD Rating Tool or expert judgment is used to determine the PD for customers in this segment</v>
-    <v>49245</v>
-    <v>Australian Securities Exchange</v>
-    <v>XASX</v>
-    <v>XASX</v>
-    <v>Ground Floor, Tower 1, 201 Sussex Street, SYDNEY, NEW SOUTH WALES, 2000 AU</v>
-    <v>109.2</v>
-    <v>Banking Services</v>
-    <v>Stock</v>
-    <v>44951.333333333336</v>
-    <v>15</v>
-    <v>107.79</v>
-    <v>182433200000</v>
-    <v>COMMONWEALTH BANK OF AUSTRALIA</v>
-    <v>COMMONWEALTH BANK OF AUSTRALIA</v>
-    <v>108.01</v>
-    <v>17.28</v>
-    <v>108.05</v>
-    <v>108.83</v>
-    <v>1688414000</v>
-    <v>CBA</v>
-    <v>COMMONWEALTH BANK OF AUSTRALIA (XASX:CBA)</v>
-    <v>1620732</v>
-    <v>2025450</v>
-    <v>1991</v>
-  </rv>
-  <rv s="2">
-    <v>16</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=aa5c2w&amp;q=XASX%3aCAT&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="4">
-    <v>7</v>
-    <v>CATAPULT GROUP INTERNATIONAL LTD (XASX:CAT)</v>
-    <v>2</v>
-    <v>8</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-AU</v>
-    <v>aa5c2w</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>1.5349999999999999</v>
-    <v>0.70499999999999996</v>
-    <v>2.4112</v>
-    <v>-2.5000000000000001E-2</v>
-    <v>-3.4247E-2</v>
-    <v>AUD</v>
-    <v>Catapult Group International Limited is an Australia-based company engaged in the development and supply of technologies that improve the performance of athletes and sports teams. The Company operates at the intersection of sports science and analytics. The Company operates through three segments: Performance &amp; Health, Tactics &amp; Coaching and Media &amp; Other. Its Performance &amp; Health segment is engaged in the design, development and supply of wearable technology and athlete monitoring software solutions to sports teams, athletes and the prosumer market. Its Tactics &amp; Coaching segment is engaged in the design, development and supply of video analysis, editing, and publishing software solutions to sports teams. Its Media &amp; Other segment provides media licensing, athlete management and professional services to customers. The Company operates through its subsidiary, Catapult Sports Inc.</v>
-    <v>Australian Securities Exchange</v>
-    <v>XASX</v>
-    <v>XASX</v>
-    <v>75 - 83 High Street, PRAHAN, VICTORIA, 3181 AU</v>
-    <v>0.73</v>
-    <v>Electronic Equipment &amp; Parts</v>
-    <v>Stock</v>
-    <v>44951.333333333336</v>
-    <v>18</v>
-    <v>0.70499999999999996</v>
-    <v>178162300</v>
-    <v>CATAPULT GROUP INTERNATIONAL LTD</v>
-    <v>CATAPULT GROUP INTERNATIONAL LTD</v>
-    <v>0.73</v>
-    <v>28.45</v>
-    <v>0.73</v>
-    <v>0.70499999999999996</v>
-    <v>244057900</v>
-    <v>CAT</v>
-    <v>CATAPULT GROUP INTERNATIONAL LTD (XASX:CAT)</v>
-    <v>95020</v>
-    <v>62270</v>
-    <v>2013</v>
-  </rv>
-  <rv s="2">
-    <v>19</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=aa658m&amp;q=XASX%3aEOS&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="1">
-    <v>0</v>
-    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED (XASX:EOS)</v>
-    <v>2</v>
-    <v>3</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-AU</v>
-    <v>aa658m</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>3.38</v>
-    <v>0.43</v>
-    <v>2.3931</v>
-    <v>-0.02</v>
-    <v>-2.8986000000000001E-2</v>
-    <v>AUD</v>
-    <v>Electro Optic Systems Holdings Limited is an Australia-based technology company. The Company’s segments include Defense Systems, Space Systems and Communications Systems. The Company’s Defense Systems develops, manufactures and markets fire control, surveillance and weapon systems to approved military customers. The Company’s Space Systems specializes in the design, manufacture, delivery and operation of sensors and systems for space domain awareness (SDA) and space control. The Company’s Communications Systems develops and provides global satellite communications products, systems and services. The Communications Systems specializes in optical, microwave and on-the-move radio and satellite systems that deliver telecommunications anywhere in the world. The Company's products incorporate electro-optic applications based on its technologies in software, laser, electronics, optronics, gimbals, telescopes and beam directors and mechanisms.</v>
-    <v>218</v>
-    <v>Australian Securities Exchange</v>
-    <v>XASX</v>
-    <v>XASX</v>
-    <v>18 Wormald Street, Symonston, AUSTRALIAN CAPITAL TERRITORY, 2609 AU</v>
-    <v>0.71</v>
-    <v>Aerospace &amp; Defense</v>
-    <v>Stock</v>
-    <v>44951.333333333336</v>
-    <v>21</v>
-    <v>0.65</v>
-    <v>118152800</v>
-    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED</v>
-    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED</v>
-    <v>0.67500000000000004</v>
-    <v>28.53</v>
-    <v>0.69</v>
-    <v>0.67</v>
-    <v>171236000</v>
-    <v>EOS</v>
-    <v>ELECTRO OPTIC SYSTEMS HOLDINGS LIMITED (XASX:EOS)</v>
-    <v>353942</v>
-    <v>700850</v>
-    <v>2000</v>
-  </rv>
-  <rv s="2">
-    <v>22</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=aa86z2&amp;q=XASX%3aNEA&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="3">
-    <v>5</v>
-    <v>NEARMAP LTD (XASX:NEA)</v>
-    <v>2</v>
-    <v>6</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-AU</v>
-    <v>aa86z2</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>2.79</v>
-    <v>1.37</v>
-    <v>1.7012</v>
-    <v>0.01</v>
-    <v>6.515E-3</v>
-    <v>AUD</v>
-    <v>Nearmap Ltd is an Australia-based location intelligence company that provides cloud-based geospatial information services. The Company's is engaged in providing online aerial photomaps to business customers via subscription through its subsidiaries, Nearmap Australia Pty Ltd and Nearmap US, Inc. The Company uses its camera systems and processing software to conduct aerial surveys that captures wide-scale urban areas in Australia, New Zealand, the United States of America, and Canada multiple times each year, making fresh content instantly available in the cloud via Web application or application programming interface (API) integration. The Company's products include Vertical Imagery, Oblique Imagery, 3D Imagery and Data, Nearmap AI, and Nearmap on OpenSolar. The Company serves various industries, including Government, construction, telecommunication, transportation, insurance, property, roofing, and solar.</v>
-    <v>400</v>
-    <v>Australian Securities Exchange</v>
-    <v>XASX</v>
-    <v>XASX</v>
-    <v>Tower 1, International Towers Sydney L 4, 100 Barangaroo Ave, SYDNEY, NEW SOUTH WALES, 2000 AU</v>
-    <v>1.57</v>
-    <v>Software &amp; IT Services</v>
-    <v>Stock</v>
-    <v>44552.02238425926</v>
-    <v>24</v>
-    <v>1.54</v>
-    <v>768177100</v>
-    <v>NEARMAP LTD</v>
-    <v>NEARMAP LTD</v>
-    <v>1.57</v>
-    <v>34.51</v>
-    <v>1.5349999999999999</v>
-    <v>1.5449999999999999</v>
-    <v>498816300</v>
-    <v>NEA</v>
-    <v>NEARMAP LTD (XASX:NEA)</v>
-    <v>509998</v>
-    <v>1998</v>
   </rv>
   <rv s="2">
     <v>25</v>
@@ -1019,6 +1009,49 @@
     <k n="%EntityId" t="s"/>
     <k n="%EntityServiceId"/>
     <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
     <k n="%OutdatedReason" t="i"/>
     <k n="%ProviderInfo" t="s"/>
     <k n="52 week high"/>
@@ -1050,49 +1083,6 @@
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
     <k n="Volume"/>
-    <k n="Year incorporated"/>
-  </s>
-  <s t="_linkedentitycore">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="_Flags" t="spb"/>
-    <k n="_Format" t="spb"/>
-    <k n="_Icon" t="s"/>
-    <k n="_SubLabel" t="spb"/>
-    <k n="%EntityCulture" t="s"/>
-    <k n="%EntityId" t="s"/>
-    <k n="%EntityServiceId"/>
-    <k n="%IsRefreshable" t="b"/>
-    <k n="%ProviderInfo" t="s"/>
-    <k n="52 week high"/>
-    <k n="52 week low"/>
-    <k n="Beta"/>
-    <k n="Change"/>
-    <k n="Change (%)"/>
-    <k n="Currency" t="s"/>
-    <k n="Description" t="s"/>
-    <k n="Exchange" t="s"/>
-    <k n="Exchange abbreviation" t="s"/>
-    <k n="ExchangeID" t="s"/>
-    <k n="Headquarters" t="s"/>
-    <k n="High"/>
-    <k n="Industry" t="s"/>
-    <k n="Instrument type" t="s"/>
-    <k n="Last trade time"/>
-    <k n="LearnMoreOnLink" t="r"/>
-    <k n="Low"/>
-    <k n="Market cap"/>
-    <k n="Name" t="s"/>
-    <k n="Official name" t="s"/>
-    <k n="Open"/>
-    <k n="P/E"/>
-    <k n="Previous close"/>
-    <k n="Price"/>
-    <k n="Shares outstanding"/>
-    <k n="Ticker symbol" t="s"/>
-    <k n="UniqueName" t="s"/>
-    <k n="Volume"/>
-    <k n="Volume average"/>
     <k n="Year incorporated"/>
   </s>
 </rvStructures>
@@ -1134,6 +1124,49 @@
       <v t="s">Shares outstanding</v>
       <v t="s">Description</v>
       <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+    <a count="41">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
       <v t="s">Headquarters</v>
       <v t="s">Industry</v>
       <v t="s">Instrument type</v>
@@ -1189,49 +1222,6 @@
       <v t="s">%ProviderInfo</v>
       <v t="s">%OutdatedReason</v>
     </a>
-    <a count="41">
-      <v t="s">%EntityServiceId</v>
-      <v t="s">_Format</v>
-      <v t="s">%IsRefreshable</v>
-      <v t="s">%EntityCulture</v>
-      <v t="s">%EntityId</v>
-      <v t="s">_Icon</v>
-      <v t="s">_Display</v>
-      <v t="s">Name</v>
-      <v t="s">_SubLabel</v>
-      <v t="s">Price</v>
-      <v t="s">Exchange</v>
-      <v t="s">Official name</v>
-      <v t="s">Last trade time</v>
-      <v t="s">Ticker symbol</v>
-      <v t="s">Exchange abbreviation</v>
-      <v t="s">Change</v>
-      <v t="s">Change (%)</v>
-      <v t="s">Currency</v>
-      <v t="s">Previous close</v>
-      <v t="s">Open</v>
-      <v t="s">High</v>
-      <v t="s">Low</v>
-      <v t="s">52 week high</v>
-      <v t="s">52 week low</v>
-      <v t="s">Volume</v>
-      <v t="s">Volume average</v>
-      <v t="s">Market cap</v>
-      <v t="s">Beta</v>
-      <v t="s">P/E</v>
-      <v t="s">Shares outstanding</v>
-      <v t="s">Description</v>
-      <v t="s">Headquarters</v>
-      <v t="s">Industry</v>
-      <v t="s">Instrument type</v>
-      <v t="s">Year incorporated</v>
-      <v t="s">_Flags</v>
-      <v t="s">UniqueName</v>
-      <v t="s">_DisplayString</v>
-      <v t="s">LearnMoreOnLink</v>
-      <v t="s">ExchangeID</v>
-      <v t="s">%ProviderInfo</v>
-    </a>
   </spbArrays>
   <spbData count="9">
     <spb s="0">
@@ -1284,6 +1274,32 @@
       <v>LearnMoreOnLink</v>
     </spb>
     <spb s="5">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="0">
+      <v>2</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="6">
       <v>10</v>
       <v>2</v>
       <v>2</v>
@@ -1299,32 +1315,6 @@
       <v>10</v>
       <v>10</v>
       <v>10</v>
-      <v>7</v>
-      <v>8</v>
-      <v>9</v>
-      <v>4</v>
-    </spb>
-    <spb s="0">
-      <v>2</v>
-      <v>Name</v>
-      <v>LearnMoreOnLink</v>
-    </spb>
-    <spb s="6">
-      <v>1</v>
-      <v>2</v>
-      <v>2</v>
-      <v>1</v>
-      <v>3</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>5</v>
-      <v>6</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
       <v>7</v>
       <v>8</v>
       <v>9</v>
@@ -1390,12 +1380,12 @@
     <k n="Price" t="i"/>
     <k n="Change" t="i"/>
     <k n="Volume" t="i"/>
-    <k n="Employees" t="i"/>
     <k n="Change (%)" t="i"/>
     <k n="Market cap" t="i"/>
     <k n="52 week low" t="i"/>
     <k n="52 week high" t="i"/>
     <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
     <k n="Last trade time" t="i"/>
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
@@ -1411,12 +1401,12 @@
     <k n="Price" t="i"/>
     <k n="Change" t="i"/>
     <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
     <k n="Change (%)" t="i"/>
     <k n="Market cap" t="i"/>
     <k n="52 week low" t="i"/>
     <k n="52 week high" t="i"/>
     <k n="Previous close" t="i"/>
-    <k n="Volume average" t="i"/>
     <k n="Last trade time" t="i"/>
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
@@ -1804,26 +1794,19 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D3" dT="2020-11-12T00:28:51.72" personId="{11AAC28B-932D-4D2E-A823-16C458804BEB}" id="{B734B965-24A6-479B-9B64-AC439E271E9A}">
-    <text>Buy, Sell, DRIP</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="3" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
     <col min="5" max="6" width="13.33203125" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" customWidth="1"/>
@@ -1833,11 +1816,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -1847,9 +1830,9 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1859,82 +1842,107 @@
       <c r="J2" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="e" cm="1" vm="1">
+        <f t="array" ref="B6:B11">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Ledger[Stock], SUMIF(Ledger[Stock], Ledger[Stock], Ledger[Units])&lt;&gt;0)))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
     <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1951,16 +1959,19 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError xmlns:x16r5="http://schemas.microsoft.com/office/spreadsheetml/2020/10/main" sqref="B11" x16r5:outdatedDataTypes="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FBC7AA-B373-4B67-A418-D04AC020DDD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FBC7AA-B373-4B67-A418-D04AC020DDD0}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2130,7 +2141,7 @@
       <c r="A8" s="1">
         <v>37155</v>
       </c>
-      <c r="B8" t="e" vm="2">
+      <c r="B8" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="C8" t="str" cm="1">
@@ -2158,7 +2169,7 @@
       <c r="A9" s="1">
         <v>43920</v>
       </c>
-      <c r="B9" t="e" vm="3">
+      <c r="B9" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="C9" t="str" cm="1">
@@ -2186,7 +2197,7 @@
       <c r="A10" s="1">
         <v>43936</v>
       </c>
-      <c r="B10" t="e" vm="3">
+      <c r="B10" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="C10" t="str" cm="1">
@@ -2214,7 +2225,7 @@
       <c r="A11" s="1">
         <v>43920</v>
       </c>
-      <c r="B11" t="e" vm="4">
+      <c r="B11" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C11" t="str" cm="1">
@@ -2242,7 +2253,7 @@
       <c r="A12" s="1">
         <v>43936</v>
       </c>
-      <c r="B12" t="e" vm="4">
+      <c r="B12" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C12" t="str" cm="1">
@@ -2270,7 +2281,7 @@
       <c r="A13" s="1">
         <v>43907</v>
       </c>
-      <c r="B13" t="e" vm="5">
+      <c r="B13" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="str" cm="1">
@@ -2298,7 +2309,7 @@
       <c r="A14" s="1">
         <v>43930</v>
       </c>
-      <c r="B14" t="e" vm="5">
+      <c r="B14" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C14" t="str" cm="1">
@@ -2326,7 +2337,7 @@
       <c r="A15" s="1">
         <v>38618</v>
       </c>
-      <c r="B15" t="e" vm="6">
+      <c r="B15" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C15" t="str" cm="1">
@@ -2354,7 +2365,7 @@
       <c r="A16" s="1">
         <v>39177</v>
       </c>
-      <c r="B16" t="e" vm="6">
+      <c r="B16" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C16" t="str" cm="1">
@@ -2382,7 +2393,7 @@
       <c r="A17" s="1">
         <v>39227</v>
       </c>
-      <c r="B17" t="e" vm="6">
+      <c r="B17" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C17" t="str" cm="1">
@@ -2410,7 +2421,7 @@
       <c r="A18" s="1">
         <v>39318</v>
       </c>
-      <c r="B18" t="e" vm="6">
+      <c r="B18" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C18" t="str" cm="1">
@@ -2438,7 +2449,7 @@
       <c r="A19" s="1">
         <v>39540</v>
       </c>
-      <c r="B19" t="e" vm="6">
+      <c r="B19" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C19" t="str" cm="1">
@@ -2466,7 +2477,7 @@
       <c r="A20" s="1">
         <v>40164</v>
       </c>
-      <c r="B20" t="e" vm="6">
+      <c r="B20" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C20" t="str" cm="1">
@@ -2494,7 +2505,7 @@
       <c r="A21" s="1">
         <v>40269</v>
       </c>
-      <c r="B21" t="e" vm="6">
+      <c r="B21" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C21" t="str" cm="1">
@@ -2522,7 +2533,7 @@
       <c r="A22" s="1">
         <v>41848</v>
       </c>
-      <c r="B22" t="e" vm="6">
+      <c r="B22" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C22" t="str" cm="1">
@@ -2553,7 +2564,7 @@
       <c r="A23" s="1">
         <v>43920</v>
       </c>
-      <c r="B23" t="e" vm="7">
+      <c r="B23" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="C23" t="str" cm="1">
@@ -2581,7 +2592,7 @@
       <c r="A24" s="1">
         <v>43920</v>
       </c>
-      <c r="B24" t="e" vm="8">
+      <c r="B24" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="C24" t="str" cm="1">
@@ -2609,7 +2620,7 @@
       <c r="A25" s="1">
         <v>43924</v>
       </c>
-      <c r="B25" t="e" vm="9">
+      <c r="B25" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="C25" t="str" cm="1">
@@ -2635,9 +2646,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added industry to dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E45D39-0AF5-5245-AF1F-B1A92E5F8215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B457F4D6-02DF-FA4B-97CD-40C7F29DD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="8720" yWindow="760" windowWidth="21520" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -1799,7 +1799,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1886,34 +1886,53 @@
         <f t="array" ref="B6:B11">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Ledger[Stock], SUMIF(Ledger[Stock], Ledger[Stock], Ledger[Units])&lt;&gt;0)))</f>
         <v>#VALUE!</v>
       </c>
+      <c r="C6" t="str" cm="1">
+        <f t="array" ref="C6:C11">_FV(_xlfn.ANCHORARRAY(B6),"Industry")</f>
+        <v>Investment Banking &amp; Investment Services</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
+      <c r="C7" t="str">
+        <v>Electronic Equipment &amp; Parts</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
+      <c r="C8" t="str">
+        <v>Banking Services</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
+      <c r="C9" t="str">
+        <v>Aerospace &amp; Defense</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
+      <c r="C10" t="str">
+        <v>Banking Services</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C11" t="str">
+        <v>Software &amp; IT Services</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added units to dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B457F4D6-02DF-FA4B-97CD-40C7F29DD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA449BFC-410E-934B-AF72-421500AA1584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8720" yWindow="760" windowWidth="21520" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -1799,7 +1799,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1890,6 +1890,10 @@
         <f t="array" ref="C6:C11">_FV(_xlfn.ANCHORARRAY(B6),"Industry")</f>
         <v>Investment Banking &amp; Investment Services</v>
       </c>
+      <c r="D6" cm="1">
+        <f t="array" ref="D6:D11">SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Units])</f>
+        <v>162</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="e" vm="2">
@@ -1898,6 +1902,9 @@
       <c r="C7" t="str">
         <v>Electronic Equipment &amp; Parts</v>
       </c>
+      <c r="D7">
+        <v>4275</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" t="e" vm="3">
@@ -1906,6 +1913,9 @@
       <c r="C8" t="str">
         <v>Banking Services</v>
       </c>
+      <c r="D8">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" t="e" vm="4">
@@ -1914,6 +1924,9 @@
       <c r="C9" t="str">
         <v>Aerospace &amp; Defense</v>
       </c>
+      <c r="D9">
+        <v>695</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" t="e" vm="5">
@@ -1922,6 +1935,9 @@
       <c r="C10" t="str">
         <v>Banking Services</v>
       </c>
+      <c r="D10">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" t="e" vm="6">
@@ -1929,6 +1945,9 @@
       </c>
       <c r="C11" t="str">
         <v>Software &amp; IT Services</v>
+      </c>
+      <c r="D11">
+        <v>1376</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added current price to dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA449BFC-410E-934B-AF72-421500AA1584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D660FCA-ED34-FF4C-B6DB-65C3CAF6747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="760" windowWidth="21520" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="7720" yWindow="760" windowWidth="21520" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -1894,6 +1894,10 @@
         <f t="array" ref="D6:D11">SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Units])</f>
         <v>162</v>
       </c>
+      <c r="E6" cm="1">
+        <f t="array" ref="E6:E11">_FV(_xlfn.ANCHORARRAY(B6),"Price")</f>
+        <v>68.569999999999993</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="e" vm="2">
@@ -1905,6 +1909,9 @@
       <c r="D7">
         <v>4275</v>
       </c>
+      <c r="E7">
+        <v>0.70499999999999996</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" t="e" vm="3">
@@ -1916,6 +1923,9 @@
       <c r="D8">
         <v>56</v>
       </c>
+      <c r="E8">
+        <v>108.83</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" t="e" vm="4">
@@ -1927,6 +1937,9 @@
       <c r="D9">
         <v>695</v>
       </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" t="e" vm="5">
@@ -1938,6 +1951,9 @@
       <c r="D10">
         <v>35</v>
       </c>
+      <c r="E10">
+        <v>31.48</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" t="e" vm="6">
@@ -1948,6 +1964,9 @@
       </c>
       <c r="D11">
         <v>1376</v>
+      </c>
+      <c r="E11">
+        <v>1.5449999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added 12 mths sparkline
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532FF214-927D-4F44-BDC9-70F1AFB2DB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57DE482-B5D7-A84E-ABCA-1CBC87C8DE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="2" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -19234,8 +19234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19525,6 +19525,44 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0774D4B0-918C-3542-A9E1-3E0F93FBA6D8}">
+          <x14:colorSeries theme="8" tint="-0.249977111117893"/>
+          <x14:colorNegative theme="9"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="9" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="9" tint="-0.249977111117893"/>
+          <x14:colorLast theme="9" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="9" tint="-0.249977111117893"/>
+          <x14:colorLow theme="9" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Last 12 Months'!B4:IS4</xm:f>
+              <xm:sqref>J6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Last 12 Months'!B5:IS5</xm:f>
+              <xm:sqref>J7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Last 12 Months'!B6:IS6</xm:f>
+              <xm:sqref>J8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Last 12 Months'!B7:IS7</xm:f>
+              <xm:sqref>J9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Last 12 Months'!B8:IS8</xm:f>
+              <xm:sqref>J10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -20191,7 +20229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7FF194-C0D9-F348-A500-237978D53721}">
   <dimension ref="A3:IS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="HX1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added total market value and today's change
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57DE482-B5D7-A84E-ABCA-1CBC87C8DE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4097FF-A57A-2542-AD59-245C151EA036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11456,7 +11456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>Ticker</t>
   </si>
@@ -11509,6 +11509,9 @@
     <t>Today's Change</t>
   </si>
   <si>
+    <t>Total Holding Market Value</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                        </t>
   </si>
   <si>
@@ -11540,7 +11543,7 @@
     <numFmt numFmtId="178" formatCode="[$$-409]#,##0.0000"/>
     <numFmt numFmtId="180" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11581,6 +11584,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -11614,7 +11638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -11623,12 +11647,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11645,6 +11667,16 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19235,7 +19267,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19252,48 +19284,58 @@
     <col min="19" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="18">
+        <f>SUM(_xlfn.ANCHORARRAY(F6))</f>
+        <v>21784.145</v>
+      </c>
+      <c r="G2" s="18">
+        <f>SUM(_xlfn.ANCHORARRAY(G6))</f>
+        <v>-149.95500000000055</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>13</v>
@@ -19312,7 +19354,7 @@
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>12</v>
@@ -19466,19 +19508,19 @@
     <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
@@ -19502,10 +19544,10 @@
     <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:J14"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:J2"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="G5:H5"/>
   </mergeCells>
@@ -20158,7 +20200,7 @@
         <v>983.04</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added icon set for percent
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4097FF-A57A-2542-AD59-245C151EA036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2344DD-EBC1-7A4B-A11C-746A6C38AEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11638,7 +11638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -11677,11 +11677,74 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -18950,16 +19013,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="7">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="19">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="16">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19267,7 +19330,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19316,7 +19379,10 @@
         <f>SUM(_xlfn.ANCHORARRAY(G6))</f>
         <v>-149.95500000000055</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="20">
+        <f>G2/(F2-G2)</f>
+        <v>-6.836615133513595E-3</v>
+      </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
@@ -19552,18 +19618,27 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G11">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I11">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added icon set for oday's change
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2344DD-EBC1-7A4B-A11C-746A6C38AEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DAEDDC-184B-A944-8B2A-75EE24D6C3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11684,7 +11684,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -19013,16 +19043,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="19">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="25">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="16">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="22">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19330,7 +19360,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19618,22 +19648,22 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G11">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H11">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I11">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="iconSet" priority="1">
+    <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -19643,6 +19673,26 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{5222772A-9D89-9D4F-B926-8BA1105DE81E}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H6:H10</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0774D4B0-918C-3542-A9E1-3E0F93FBA6D8}">

</xml_diff>

<commit_message>
Added data bars for market value
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DAEDDC-184B-A944-8B2A-75EE24D6C3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF73B895-7D09-2E45-9E8B-D97D92C3895A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11647,10 +11647,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11664,13 +11666,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11680,11 +11678,53 @@
     <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -19043,16 +19083,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="31">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="28">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -19360,21 +19400,21 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="18" width="10.83203125" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" hidden="1"/>
+    <col min="1" max="1" width="2.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="6" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" style="6" customWidth="1"/>
+    <col min="11" max="18" width="10.83203125" style="6" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="6" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -19383,51 +19423,51 @@
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="16" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="18">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="14">
         <f>SUM(_xlfn.ANCHORARRAY(F6))</f>
         <v>21784.145</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="14">
         <f>SUM(_xlfn.ANCHORARRAY(G6))</f>
         <v>-149.95500000000055</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="16">
         <f>G2/(F2-G2)</f>
         <v>-6.836615133513595E-3</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
@@ -19457,166 +19497,166 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" t="e" cm="1" vm="1">
+      <c r="B6" s="6" t="e" cm="1" vm="1">
         <f t="array" ref="B6:B10">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Ledger[Stock], SUMIF(Ledger[Stock], Ledger[Stock], Ledger[Units])&lt;&gt;0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C6" t="str" cm="1">
+      <c r="C6" s="6" t="str" cm="1">
         <f t="array" ref="C6:C10">_FV(_xlfn.ANCHORARRAY(B6),"Industry")</f>
         <v>Investment Banking &amp; Investment Services</v>
       </c>
-      <c r="D6" cm="1">
+      <c r="D6" s="6" cm="1">
         <f t="array" ref="D6:D10">SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Units])</f>
         <v>162</v>
       </c>
-      <c r="E6" s="13" cm="1">
+      <c r="E6" s="19" cm="1">
         <f t="array" ref="E6:E10">_FV(_xlfn.ANCHORARRAY(B6),"Price")</f>
         <v>68.569999999999993</v>
       </c>
-      <c r="F6" s="13" cm="1">
+      <c r="F6" s="19" cm="1">
         <f t="array" ref="F6:F10">_xlfn.ANCHORARRAY(D6)*_xlfn.ANCHORARRAY(E6)</f>
         <v>11108.339999999998</v>
       </c>
-      <c r="G6" s="14" cm="1">
+      <c r="G6" s="19" cm="1">
         <f t="array" ref="G6:G10">(_xlfn.ANCHORARRAY(E6)-_FV(_xlfn.ANCHORARRAY(B6),"Previous close",TRUE))*_xlfn.ANCHORARRAY(D6)</f>
         <v>-77.760000000000645</v>
       </c>
-      <c r="H6" s="15" cm="1">
+      <c r="H6" s="20" cm="1">
         <f t="array" ref="H6:H10">_xlfn.ANCHORARRAY(G6)/(_xlfn.ANCHORARRAY(F6)-_xlfn.ANCHORARRAY(G6))</f>
         <v>-6.9514844315713836E-3</v>
       </c>
-      <c r="I6" s="13" cm="1">
+      <c r="I6" s="19" cm="1">
         <f t="array" ref="I6:I10">-SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Transaction Amount])+_xlfn.ANCHORARRAY(F6)</f>
         <v>6038.2099999999991</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" t="e" vm="2">
+      <c r="B7" s="6" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="6" t="str">
         <v>Electronic Equipment &amp; Parts</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>4275</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="19">
         <v>0.70499999999999996</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="19">
         <v>3013.875</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="19">
         <v>-106.8750000000001</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="20">
         <v>-3.4246575342465786E-2</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="19">
         <v>320.625</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" t="e" vm="3">
+      <c r="B8" s="6" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="6" t="str">
         <v>Banking Services</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>56</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="19">
         <v>108.83</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="19">
         <v>6094.48</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="19">
         <v>43.680000000000064</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="20">
         <v>7.2188801480796046E-3</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="19">
         <v>3345.55</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" t="e" vm="4">
+      <c r="B9" s="6" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="6" t="str">
         <v>Aerospace &amp; Defense</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>695</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="19">
         <v>0.67</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="19">
         <v>465.65000000000003</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="19">
         <v>-13.899999999999935</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="20">
         <v>-2.8985507246376677E-2</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="19">
         <v>-2237.9</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" t="e" vm="5">
+      <c r="B10" s="6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="6" t="str">
         <v>Banking Services</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>35</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="19">
         <v>31.48</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="19">
         <v>1101.8</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="19">
         <v>4.9000000000000199</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="20">
         <v>4.4671346522016783E-3</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="19">
         <v>139.64999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="13"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
@@ -19634,10 +19674,10 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G1:H1"/>
@@ -19648,22 +19688,22 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H11">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I11">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -19671,12 +19711,26 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F10">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="8" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{40FBD065-52FC-7643-BAF0-721A17AE6CD1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{5222772A-9D89-9D4F-B926-8BA1105DE81E}">
+          <x14:cfRule type="iconSet" priority="2" id="{5222772A-9D89-9D4F-B926-8BA1105DE81E}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -19690,6 +19744,19 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>H6:H10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{40FBD065-52FC-7643-BAF0-721A17AE6CD1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor theme="8" tint="-0.249977111117893"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F6:F10</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added exc rate indicator
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B93342-2A1F-7A4D-932C-D30A0EC6351F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE4E71B-E160-A847-A6B9-4448992ECCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="6940" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -11698,7 +11698,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13523,18 +13523,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.0500000000000001E-2</v>
-    <v>-7.4009999999999996E-3</v>
+    <v>-1.0699999999999999E-2</v>
+    <v>-7.5420000000000001E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.795567129629</v>
+    <v>44951.799155092594</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4083000000000001</v>
+    <v>1.4080999999999999</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -19611,9 +19611,9 @@
         <f>SUM(_xlfn.ANCHORARRAY(I6))</f>
         <v>7606.1349999999984</v>
       </c>
-      <c r="J2" s="21" cm="1">
-        <f t="array" ref="J2">_FV(J1,"Price")</f>
-        <v>1.4083000000000001</v>
+      <c r="J2" s="21" t="str" cm="1">
+        <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
+        <v>$1.4081▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added portfolio by industry
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE4E71B-E160-A847-A6B9-4448992ECCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5054A74F-728D-FF48-A3DD-8E35DCD8A1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="8340" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -19550,7 +19550,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19833,11 +19833,41 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="str" cm="1">
+        <f t="array" ref="B16:B19">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(C6))</f>
+        <v>Investment Banking &amp; Investment Services</v>
+      </c>
+      <c r="C16" s="19" cm="1">
+        <f t="array" ref="C16:C19">SUMIF(_xlfn.ANCHORARRAY(C6),_xlfn.ANCHORARRAY( B16),_xlfn.ANCHORARRAY( F6))</f>
+        <v>11108.339999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="str">
+        <v>Electronic Equipment &amp; Parts</v>
+      </c>
+      <c r="C17" s="19">
+        <v>3013.875</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="str">
+        <v>Banking Services</v>
+      </c>
+      <c r="C18" s="19">
+        <v>7196.28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="str">
+        <v>Aerospace &amp; Defense</v>
+      </c>
+      <c r="C19" s="19">
+        <v>465.65000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
Added watchlist exchange and ticker
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B07B4B4-52D7-9F47-B78C-65581844EF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A70DD3-47BF-194E-BC0D-B83C47E64A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11487,7 +11487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Ticker</t>
   </si>
@@ -11531,6 +11531,9 @@
     <t>Industry</t>
   </si>
   <si>
+    <t>Exchange</t>
+  </si>
+  <si>
     <t>Market Value</t>
   </si>
   <si>
@@ -11565,6 +11568,9 @@
   </si>
   <si>
     <t>Unrealised Gain/Loss</t>
+  </si>
+  <si>
+    <t>Ticker symbol</t>
   </si>
 </sst>
 </file>
@@ -11725,37 +11731,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -20495,16 +20471,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="37">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="31">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="34">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="28">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20513,10 +20489,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:A4" totalsRowShown="0">
-  <autoFilter ref="A2:A4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:C4" totalsRowShown="0">
+  <autoFilter ref="A2:C4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4F0E7149-3BD7-2845-9C01-D309308BCAE4}" name="Stock"/>
+    <tableColumn id="2" xr3:uid="{141EDC37-F4ED-4846-A2CA-BA1968670B3E}" name="Exchange">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Exchange")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C1DB10F8-98A9-6F48-AB57-FA11A36AFB9A}" name="Ticker symbol">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20841,21 +20823,21 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="H1" s="15"/>
       <c r="I1" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J1" s="16" t="e" vm="1">
         <v>#VALUE!</v>
@@ -20890,7 +20872,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -20903,7 +20885,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>13</v>
@@ -20915,14 +20897,14 @@
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>12</v>
@@ -21077,11 +21059,11 @@
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -21095,7 +21077,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -21345,7 +21327,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21880,7 +21862,7 @@
         <v>983.04</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -28043,30 +28025,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="e" vm="1141">
         <v>#VALUE!</v>
       </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_FV(Table2[[#This Row],[Stock]],"Exchange")</f>
+        <v>Australian Securities Exchange</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" ref="C3">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
+        <v>BLD</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="e" vm="1142">
         <v>#VALUE!</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">_FV(Table2[[#This Row],[Stock]],"Exchange")</f>
+        <v>Australian Securities Exchange</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
+        <v>ASB</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added watchlist 52 weeks high/low and price
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A70DD3-47BF-194E-BC0D-B83C47E64A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54854C9-6A79-1C49-B4EF-25478E3016B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11487,7 +11487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Ticker</t>
   </si>
@@ -11572,14 +11572,21 @@
   <si>
     <t>Ticker symbol</t>
   </si>
+  <si>
+    <t>52 week high</t>
+  </si>
+  <si>
+    <t>52 week low</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$$-409]#,##0.0000"/>
     <numFmt numFmtId="180" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="181" formatCode="_-[$$-C09]* #,##0.0000_-;\-[$$-C09]* #,##0.0000_-;_-[$$-C09]* &quot;-&quot;????_-;_-@_-"/>
@@ -11672,7 +11679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -11727,100 +11734,20 @@
     <xf numFmtId="181" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="18">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -14659,18 +14586,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.15E-2</v>
-    <v>-8.1049999999999994E-3</v>
+    <v>-1.0500000000000001E-2</v>
+    <v>-7.4009999999999996E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.806643518517</v>
+    <v>44951.810196759259</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4073</v>
+    <v>1.4083000000000001</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -20471,16 +20398,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="31">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="16">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="28">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="13">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20489,15 +20416,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:C4" totalsRowShown="0">
-  <autoFilter ref="A2:C4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:F4" totalsRowShown="0">
+  <autoFilter ref="A2:F4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4F0E7149-3BD7-2845-9C01-D309308BCAE4}" name="Stock"/>
     <tableColumn id="2" xr3:uid="{141EDC37-F4ED-4846-A2CA-BA1968670B3E}" name="Exchange">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Exchange")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C1DB10F8-98A9-6F48-AB57-FA11A36AFB9A}" name="Ticker symbol">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E5DDF0CF-5A2E-7A41-ADB8-EE3D71BF83EE}" name="52 week high" dataDxfId="2">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{AFDB2F2A-A0D4-A042-827D-78260864DF6D}" name="52 week low" dataDxfId="1">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{DC89D1B8-40CD-9F4C-A2AD-83C2E9A48094}" name="Price" dataDxfId="0">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Price")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -20867,7 +20803,7 @@
       </c>
       <c r="J2" s="21" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4073▼</v>
+        <v>$1.4083▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -21132,17 +21068,17 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G11">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H11">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I11">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28025,10 +27961,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28036,9 +27972,11 @@
     <col min="1" max="1" width="53.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -28048,8 +27986,17 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="e" vm="1141">
         <v>#VALUE!</v>
       </c>
@@ -28061,8 +28008,20 @@
         <f t="array" ref="C3">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
         <v>BLD</v>
       </c>
+      <c r="D3" s="22" cm="1">
+        <f t="array" ref="D3">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</f>
+        <v>4.17</v>
+      </c>
+      <c r="E3" s="22" cm="1">
+        <f t="array" ref="E3">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</f>
+        <v>2.48</v>
+      </c>
+      <c r="F3" s="22" cm="1">
+        <f t="array" ref="F3">_FV(Table2[[#This Row],[Stock]],"Price")</f>
+        <v>3.56</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="e" vm="1142">
         <v>#VALUE!</v>
       </c>
@@ -28073,6 +28032,18 @@
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
         <v>ASB</v>
+      </c>
+      <c r="D4" s="22" cm="1">
+        <f t="array" ref="D4">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</f>
+        <v>2.82</v>
+      </c>
+      <c r="E4" s="22" cm="1">
+        <f t="array" ref="E4">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</f>
+        <v>1.69</v>
+      </c>
+      <c r="F4" s="22" cm="1">
+        <f t="array" ref="F4">_FV(Table2[[#This Row],[Stock]],"Price")</f>
+        <v>1.6950000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added watchlist p/e and change
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54854C9-6A79-1C49-B4EF-25478E3016B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC7D4E-EE5B-7D43-885B-E934C8321930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -11487,7 +11487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>Ticker</t>
   </si>
@@ -11529,6 +11529,12 @@
   </si>
   <si>
     <t>Industry</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
   <si>
     <t>Exchange</t>
@@ -11739,7 +11745,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -20398,16 +20410,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="18">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="15">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20416,9 +20428,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:F4" totalsRowShown="0">
-  <autoFilter ref="A2:F4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}" name="Table2" displayName="Table2" ref="A2:H4" totalsRowShown="0">
+  <autoFilter ref="A2:H4" xr:uid="{D050EDB4-2AF3-9446-8843-4B09AB05FC35}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4F0E7149-3BD7-2845-9C01-D309308BCAE4}" name="Stock"/>
     <tableColumn id="2" xr3:uid="{141EDC37-F4ED-4846-A2CA-BA1968670B3E}" name="Exchange">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Exchange")</calculatedColumnFormula>
@@ -20426,14 +20438,20 @@
     <tableColumn id="3" xr3:uid="{C1DB10F8-98A9-6F48-AB57-FA11A36AFB9A}" name="Ticker symbol">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E5DDF0CF-5A2E-7A41-ADB8-EE3D71BF83EE}" name="52 week high" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{E5DDF0CF-5A2E-7A41-ADB8-EE3D71BF83EE}" name="52 week high" dataDxfId="4">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{AFDB2F2A-A0D4-A042-827D-78260864DF6D}" name="52 week low" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{AFDB2F2A-A0D4-A042-827D-78260864DF6D}" name="52 week low" dataDxfId="3">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC89D1B8-40CD-9F4C-A2AD-83C2E9A48094}" name="Price" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{DC89D1B8-40CD-9F4C-A2AD-83C2E9A48094}" name="Price" dataDxfId="2">
       <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Price")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{52B69A08-7AE3-334D-9323-0FECD393BECF}" name="P/E" dataDxfId="1">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"P/E",TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{38775435-72C5-264B-9238-5198F91F66AD}" name="Change" dataDxfId="0">
+      <calculatedColumnFormula array="1">_FV(Table2[[#This Row],[Stock]],"Change")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -20759,21 +20777,21 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" s="15"/>
       <c r="I1" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" s="16" t="e" vm="1">
         <v>#VALUE!</v>
@@ -20808,7 +20826,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -20821,7 +20839,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>13</v>
@@ -20833,14 +20851,14 @@
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>12</v>
@@ -20995,11 +21013,11 @@
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -21013,7 +21031,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -21068,17 +21086,17 @@
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G11">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H11">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I11">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21263,7 +21281,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21798,7 +21816,7 @@
         <v>983.04</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -27961,7 +27979,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -27976,27 +27994,33 @@
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="e" vm="1141">
         <v>#VALUE!</v>
       </c>
@@ -28020,8 +28044,16 @@
         <f t="array" ref="F3">_FV(Table2[[#This Row],[Stock]],"Price")</f>
         <v>3.56</v>
       </c>
+      <c r="G3" s="22" cm="1">
+        <f t="array" ref="G3">_FV(Table2[[#This Row],[Stock]],"P/E",TRUE)</f>
+        <v>3.97</v>
+      </c>
+      <c r="H3" s="22" cm="1">
+        <f t="array" ref="H3">_FV(Table2[[#This Row],[Stock]],"Change")</f>
+        <v>0.11</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="e" vm="1142">
         <v>#VALUE!</v>
       </c>
@@ -28044,6 +28076,14 @@
       <c r="F4" s="22" cm="1">
         <f t="array" ref="F4">_FV(Table2[[#This Row],[Stock]],"Price")</f>
         <v>1.6950000000000001</v>
+      </c>
+      <c r="G4" s="22" cm="1">
+        <f t="array" ref="G4">_FV(Table2[[#This Row],[Stock]],"P/E",TRUE)</f>
+        <v>8.02</v>
+      </c>
+      <c r="H4" s="22" cm="1">
+        <f t="array" ref="H4">_FV(Table2[[#This Row],[Stock]],"Change")</f>
+        <v>-7.0000000000000007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added watchlist pivot table
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC7D4E-EE5B-7D43-885B-E934C8321930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366279C9-9017-2245-9CC9-D95E5242AA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <definedName name="stock_chart_data">_xlfn.STOCKHISTORY(#REF!&amp;":"&amp;#REF!,TODAY()-30,TODAY(),0,1,0,5,2,3,4,1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="8" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -11487,7 +11490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>Ticker</t>
   </si>
@@ -11540,6 +11543,15 @@
     <t>Exchange</t>
   </si>
   <si>
+    <t>ASB</t>
+  </si>
+  <si>
+    <t>BLD</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
     <t>Market Value</t>
   </si>
   <si>
@@ -11583,6 +11595,9 @@
   </si>
   <si>
     <t>52 week low</t>
+  </si>
+  <si>
+    <t>Australian Securities Exchange</t>
   </si>
 </sst>
 </file>
@@ -11685,11 +11700,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12949,6 +12965,181 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44952.062297569442" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{B795B832-AD6F-2E49-839A-507D90445749}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table2"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Stock" numFmtId="0">
+      <sharedItems count="2">
+        <s v="BORAL LIMITED (XASX:BLD)"/>
+        <s v="AUSTAL LIMITED (XASX:ASB)"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Exchange" numFmtId="0">
+      <sharedItems count="1">
+        <s v="Australian Securities Exchange"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Ticker symbol" numFmtId="0">
+      <sharedItems count="2">
+        <s v="BLD"/>
+        <s v="ASB"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="52 week high" numFmtId="177">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.82" maxValue="4.17"/>
+    </cacheField>
+    <cacheField name="52 week low" numFmtId="177">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.69" maxValue="2.48"/>
+    </cacheField>
+    <cacheField name="Price" numFmtId="177">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.6950000000000001" maxValue="3.56"/>
+    </cacheField>
+    <cacheField name="P/E" numFmtId="177">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.97" maxValue="8.02"/>
+    </cacheField>
+    <cacheField name="Change" numFmtId="177">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-7.0000000000000007E-2" maxValue="0.11"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.17"/>
+    <n v="2.48"/>
+    <n v="3.56"/>
+    <n v="3.97"/>
+    <n v="0.11"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2.82"/>
+    <n v="1.69"/>
+    <n v="1.6950000000000001"/>
+    <n v="8.02"/>
+    <n v="-7.0000000000000007E-2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A11:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20763,315 +20954,315 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="6" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="6" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" style="6" customWidth="1"/>
-    <col min="11" max="18" width="10.83203125" style="6" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="6" hidden="1"/>
+    <col min="1" max="1" width="2.83203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="7" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" style="7" customWidth="1"/>
+    <col min="11" max="18" width="10.83203125" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="7" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="16" t="e" vm="1">
+      <c r="H1" s="16"/>
+      <c r="I1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="17" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="14">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="15">
         <f>SUM(_xlfn.ANCHORARRAY(F6))</f>
         <v>21784.145</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="15">
         <f>SUM(_xlfn.ANCHORARRAY(G6))</f>
         <v>-149.95500000000055</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="18">
         <f>G2/(F2-G2)</f>
         <v>-6.836615133513595E-3</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="15">
         <f>SUM(_xlfn.ANCHORARRAY(I6))</f>
         <v>7606.1349999999984</v>
       </c>
-      <c r="J2" s="21" t="str" cm="1">
+      <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
         <v>$1.4083▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="10" t="s">
+      <c r="F5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="e" cm="1" vm="2">
+      <c r="B6" s="7" t="e" cm="1" vm="2">
         <f t="array" ref="B6:B10">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Ledger[Stock], SUMIF(Ledger[Stock], Ledger[Stock], Ledger[Units])&lt;&gt;0)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C6" s="6" t="str" cm="1">
+      <c r="C6" s="7" t="str" cm="1">
         <f t="array" ref="C6:C10">_FV(_xlfn.ANCHORARRAY(B6),"Industry")</f>
         <v>Investment Banking &amp; Investment Services</v>
       </c>
-      <c r="D6" s="6" cm="1">
+      <c r="D6" s="7" cm="1">
         <f t="array" ref="D6:D10">SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Units])</f>
         <v>162</v>
       </c>
-      <c r="E6" s="19" cm="1">
+      <c r="E6" s="20" cm="1">
         <f t="array" ref="E6:E10">_FV(_xlfn.ANCHORARRAY(B6),"Price")</f>
         <v>68.569999999999993</v>
       </c>
-      <c r="F6" s="19" cm="1">
+      <c r="F6" s="20" cm="1">
         <f t="array" ref="F6:F10">_xlfn.ANCHORARRAY(D6)*_xlfn.ANCHORARRAY(E6)</f>
         <v>11108.339999999998</v>
       </c>
-      <c r="G6" s="19" cm="1">
+      <c r="G6" s="20" cm="1">
         <f t="array" ref="G6:G10">(_xlfn.ANCHORARRAY(E6)-_FV(_xlfn.ANCHORARRAY(B6),"Previous close",TRUE))*_xlfn.ANCHORARRAY(D6)</f>
         <v>-77.760000000000645</v>
       </c>
-      <c r="H6" s="20" cm="1">
+      <c r="H6" s="21" cm="1">
         <f t="array" ref="H6:H10">_xlfn.ANCHORARRAY(G6)/(_xlfn.ANCHORARRAY(F6)-_xlfn.ANCHORARRAY(G6))</f>
         <v>-6.9514844315713836E-3</v>
       </c>
-      <c r="I6" s="19" cm="1">
+      <c r="I6" s="20" cm="1">
         <f t="array" ref="I6:I10">-SUMIF(Ledger[Stock],_xlfn.ANCHORARRAY( B6), Ledger[Transaction Amount])+_xlfn.ANCHORARRAY(F6)</f>
         <v>6038.2099999999991</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="e" vm="3">
+      <c r="B7" s="7" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="7" t="str">
         <v>Electronic Equipment &amp; Parts</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>4275</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="20">
         <v>0.70499999999999996</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="20">
         <v>3013.875</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="20">
         <v>-106.8750000000001</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="21">
         <v>-3.4246575342465786E-2</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="20">
         <v>320.625</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="e" vm="4">
+      <c r="B8" s="7" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="C8" s="6" t="str">
+      <c r="C8" s="7" t="str">
         <v>Banking Services</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>56</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="20">
         <v>108.83</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="20">
         <v>6094.48</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="20">
         <v>43.680000000000064</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="21">
         <v>7.2188801480796046E-3</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="20">
         <v>3345.55</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="e" vm="5">
+      <c r="B9" s="7" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="7" t="str">
         <v>Aerospace &amp; Defense</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>695</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="20">
         <v>0.67</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="20">
         <v>465.65000000000003</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="20">
         <v>-13.899999999999935</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="21">
         <v>-2.8985507246376677E-2</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="20">
         <v>-2237.9</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="e" vm="6">
+      <c r="B10" s="7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="7" t="str">
         <v>Banking Services</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <v>35</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="20">
         <v>31.48</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="20">
         <v>1101.8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="20">
         <v>4.9000000000000199</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="21">
         <v>4.4671346522016783E-3</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="20">
         <v>139.64999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="str" cm="1">
+      <c r="B16" s="7" t="str" cm="1">
         <f t="array" ref="B16:B19">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(C6))</f>
         <v>Investment Banking &amp; Investment Services</v>
       </c>
-      <c r="C16" s="19" cm="1">
+      <c r="C16" s="20" cm="1">
         <f t="array" ref="C16:C19">SUMIF(_xlfn.ANCHORARRAY(C6),_xlfn.ANCHORARRAY( B16),_xlfn.ANCHORARRAY( F6))</f>
         <v>11108.339999999998</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="str">
+      <c r="B17" s="7" t="str">
         <v>Electronic Equipment &amp; Parts</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="20">
         <v>3013.875</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="str">
+      <c r="B18" s="7" t="str">
         <v>Banking Services</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="20">
         <v>7196.28</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="str">
+      <c r="B19" s="7" t="str">
         <v>Aerospace &amp; Defense</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="20">
         <v>465.65000000000003</v>
       </c>
     </row>
@@ -21256,7 +21447,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K1" s="5"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -21281,7 +21472,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21301,10 +21492,10 @@
       <c r="E4" s="3">
         <v>150</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="13">
         <v>32.21</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="2">
@@ -21329,10 +21520,10 @@
       <c r="E5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="13">
         <v>31.33</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2">
@@ -21357,10 +21548,10 @@
       <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="13">
         <v>5.44</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="2">
@@ -21385,10 +21576,10 @@
       <c r="E7" s="3">
         <v>4</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="13">
         <v>29.36</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="2">
@@ -21413,10 +21604,10 @@
       <c r="E8" s="3">
         <v>35</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="13">
         <v>27.49</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="2">
@@ -21441,10 +21632,10 @@
       <c r="E9" s="3">
         <v>274</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="13">
         <v>9.85</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="2">
@@ -21469,10 +21660,10 @@
       <c r="E10" s="3">
         <v>-274</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="13">
         <v>11.06</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="2">
@@ -21497,10 +21688,10 @@
       <c r="E11" s="3">
         <v>385</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="13">
         <v>6.99</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="2">
@@ -21525,10 +21716,10 @@
       <c r="E12" s="3">
         <v>-385</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="13">
         <v>8.15</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="2">
@@ -21553,10 +21744,10 @@
       <c r="E13" s="3">
         <v>8400</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="13">
         <v>3.52</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="2">
@@ -21581,10 +21772,10 @@
       <c r="E14" s="3">
         <v>-8400</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="13">
         <v>3.34</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="2">
@@ -21609,10 +21800,10 @@
       <c r="E15" s="3">
         <v>35</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="13">
         <v>37.19</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="2">
@@ -21637,10 +21828,10 @@
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="13">
         <v>50.02</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2">
@@ -21665,10 +21856,10 @@
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="13">
         <v>55.35</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="2">
@@ -21693,10 +21884,10 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="13">
         <v>54.8</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="2">
@@ -21721,10 +21912,10 @@
       <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="13">
         <v>39.44</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="2">
@@ -21749,10 +21940,10 @@
       <c r="E20" s="3">
         <v>3</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="13">
         <v>52.09</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H20" s="2">
@@ -21777,10 +21968,10 @@
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="13">
         <v>53.56</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="2">
@@ -21805,10 +21996,10 @@
       <c r="E22" s="3">
         <v>12</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="13">
         <v>81.92</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="2">
@@ -21816,7 +22007,7 @@
         <v>983.04</v>
       </c>
       <c r="J22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -21836,10 +22027,10 @@
       <c r="E23" s="3">
         <v>4275</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="13">
         <v>0.63</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="2">
@@ -21864,10 +22055,10 @@
       <c r="E24" s="3">
         <v>695</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="13">
         <v>3.89</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="2">
@@ -27979,16 +28170,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
-  <dimension ref="A2:H4"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
@@ -28002,13 +28193,13 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -28032,23 +28223,23 @@
         <f t="array" ref="C3">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
         <v>BLD</v>
       </c>
-      <c r="D3" s="22" cm="1">
+      <c r="D3" s="23" cm="1">
         <f t="array" ref="D3">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</f>
         <v>4.17</v>
       </c>
-      <c r="E3" s="22" cm="1">
+      <c r="E3" s="23" cm="1">
         <f t="array" ref="E3">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</f>
         <v>2.48</v>
       </c>
-      <c r="F3" s="22" cm="1">
+      <c r="F3" s="23" cm="1">
         <f t="array" ref="F3">_FV(Table2[[#This Row],[Stock]],"Price")</f>
         <v>3.56</v>
       </c>
-      <c r="G3" s="22" cm="1">
+      <c r="G3" s="23" cm="1">
         <f t="array" ref="G3">_FV(Table2[[#This Row],[Stock]],"P/E",TRUE)</f>
         <v>3.97</v>
       </c>
-      <c r="H3" s="22" cm="1">
+      <c r="H3" s="23" cm="1">
         <f t="array" ref="H3">_FV(Table2[[#This Row],[Stock]],"Change")</f>
         <v>0.11</v>
       </c>
@@ -28065,31 +28256,63 @@
         <f t="array" ref="C4">_FV(Table2[[#This Row],[Stock]],"Ticker symbol",TRUE)</f>
         <v>ASB</v>
       </c>
-      <c r="D4" s="22" cm="1">
+      <c r="D4" s="23" cm="1">
         <f t="array" ref="D4">_FV(Table2[[#This Row],[Stock]],"52 week high",TRUE)</f>
         <v>2.82</v>
       </c>
-      <c r="E4" s="22" cm="1">
+      <c r="E4" s="23" cm="1">
         <f t="array" ref="E4">_FV(Table2[[#This Row],[Stock]],"52 week low",TRUE)</f>
         <v>1.69</v>
       </c>
-      <c r="F4" s="22" cm="1">
+      <c r="F4" s="23" cm="1">
         <f t="array" ref="F4">_FV(Table2[[#This Row],[Stock]],"Price")</f>
         <v>1.6950000000000001</v>
       </c>
-      <c r="G4" s="22" cm="1">
+      <c r="G4" s="23" cm="1">
         <f t="array" ref="G4">_FV(Table2[[#This Row],[Stock]],"P/E",TRUE)</f>
         <v>8.02</v>
       </c>
-      <c r="H4" s="22" cm="1">
+      <c r="H4" s="23" cm="1">
         <f t="array" ref="H4">_FV(Table2[[#This Row],[Stock]],"Change")</f>
         <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added stock filter pages
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366279C9-9017-2245-9CC9-D95E5242AA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964BEBC0-E247-8E4B-A11B-EEA3DF520329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="4" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
     <sheet name="Ledger" sheetId="2" r:id="rId2"/>
     <sheet name="Last 12 Months" sheetId="17" r:id="rId3"/>
-    <sheet name="Watchlist" sheetId="18" r:id="rId4"/>
+    <sheet name="ASB" sheetId="20" r:id="rId4"/>
+    <sheet name="BLD" sheetId="19" r:id="rId5"/>
+    <sheet name="Watchlist" sheetId="18" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlcn.WorksheetConnection_InfoB6B7" hidden="1">#REF!</definedName>
@@ -24,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -11490,7 +11492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>Ticker</t>
   </si>
@@ -11538,6 +11540,12 @@
   </si>
   <si>
     <t>Change</t>
+  </si>
+  <si>
+    <t>AUSTAL LIMITED (XASX:ASB)</t>
+  </si>
+  <si>
+    <t>BORAL LIMITED (XASX:BLD)</t>
   </si>
   <si>
     <t>Exchange</t>
@@ -11761,7 +11769,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="14">
     <dxf>
       <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -11776,36 +11784,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="177" formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -13040,6 +13018,206 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x/>
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" item="0" hier="-1"/>
+  </pageFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="177" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x/>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" item="1" hier="-1"/>
+  </pageFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A11:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
@@ -14789,18 +14967,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.0500000000000001E-2</v>
-    <v>-7.4009999999999996E-3</v>
+    <v>-1.03E-2</v>
+    <v>-7.26E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.810196759259</v>
+    <v>44951.813923611109</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4083000000000001</v>
+    <v>1.4085000000000001</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -20601,16 +20779,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5458C81D-CC10-4A26-B7E5-A6C2BA30B3FE}" name="Ledger" displayName="Ledger" ref="A3:H24" totalsRowShown="0">
   <autoFilter ref="A3:H24" xr:uid="{69CD7EF4-09A9-4E37-9AFA-74C63E7BE9A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{92DC7DDF-D80B-405C-9573-2B90B2FF3DC9}" name="Date" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{1C907D3F-AD8C-47AB-92A9-7C471B9EBC2B}" name="Stock"/>
-    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{9CA9E601-F4B2-4F5A-B219-70B237E1CACC}" name="Ticker" dataDxfId="12">
       <calculatedColumnFormula array="1">_FV(Ledger[[#This Row],[Stock]],"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AB1CAC5C-55FF-4BD4-86DE-2DFDA8FCCD7E}" name="Transaction"/>
-    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{1B8E9E3F-3260-4B15-A698-12A2A91FCBD0}" name="Units" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{182E21A3-DB2D-4267-9431-E3760942B4C8}" name="Price" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{412DB4B2-0FAB-4830-ABAF-3EB7A6F10571}" name="Currency" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{DC43D3F6-96CE-4588-B592-F71E50711807}" name="Transaction Amount" dataDxfId="9">
       <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20968,21 +21146,21 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J1" s="17" t="e" vm="1">
         <v>#VALUE!</v>
@@ -21012,12 +21190,12 @@
       </c>
       <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4083▼</v>
+        <v>$1.4085▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -21030,7 +21208,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>13</v>
@@ -21042,14 +21220,14 @@
         <v>11</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>12</v>
@@ -21204,11 +21382,11 @@
     <row r="13" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -21222,7 +21400,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -21472,7 +21650,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22007,7 +22185,7 @@
         <v>983.04</v>
       </c>
       <c r="J22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -28169,17 +28347,98 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A53158-39AD-6F4A-9FB2-AE17C2A023A7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33D8CFE-9DEC-4C44-9F11-E2A67B5A6207}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
   <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
@@ -28190,16 +28449,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -28282,31 +28541,31 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stockhistory for ASB
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC92FFB-17BF-2841-95F5-6A6F8C271F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595BBE5F-03D0-8F46-B19D-B09C9BC35304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="5" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="7980" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
     <sheet name="Ledger" sheetId="2" r:id="rId2"/>
     <sheet name="Last 12 Months" sheetId="17" r:id="rId3"/>
-    <sheet name="ASB" sheetId="20" r:id="rId4"/>
-    <sheet name="BLD" sheetId="19" r:id="rId5"/>
+    <sheet name="ASB" sheetId="22" r:id="rId4"/>
+    <sheet name="BLD" sheetId="21" r:id="rId5"/>
     <sheet name="Watchlist" sheetId="18" r:id="rId6"/>
   </sheets>
   <definedNames>
@@ -59,7 +59,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1142">
+  <futureMetadata name="XLRICHVALUE" count="1233">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -8043,6 +8043,20 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1157"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1158"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1159"/>
         </ext>
       </extLst>
@@ -8050,7 +8064,630 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1160"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1161"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1162"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1163"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1164"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1165"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1166"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1167"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1168"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1169"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1170"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1171"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1172"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1173"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1174"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1175"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1176"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1177"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1178"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1179"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1180"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1181"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1182"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1183"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1184"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1185"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1186"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1187"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1188"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1189"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1190"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1191"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1192"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1193"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1194"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1195"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1196"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1197"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1198"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1199"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1200"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1201"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1202"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1203"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1204"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1205"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1206"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1207"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1208"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1209"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1210"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1211"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1212"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1213"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1214"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1215"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1216"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1217"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1218"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1219"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1220"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1221"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1222"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1223"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1224"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1225"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1226"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1227"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1228"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1229"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1230"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1231"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1232"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1233"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1234"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1235"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1236"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1237"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1238"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1239"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1240"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1241"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1242"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1243"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1244"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1245"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1246"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1247"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1250"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1253"/>
         </ext>
       </extLst>
     </bk>
@@ -8060,7 +8697,7 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1142">
+  <valueMetadata count="1233">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -11486,13 +12123,286 @@
     </bk>
     <bk>
       <rc t="2" v="1141"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1142"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1143"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1144"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1145"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1146"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1147"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1148"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1149"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1150"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1151"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1152"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1153"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1154"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1155"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1156"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1157"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1158"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1159"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1160"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1161"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1162"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1163"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1164"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1165"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1166"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1167"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1168"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1169"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1170"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1171"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1172"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1173"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1174"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1175"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1176"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1177"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1178"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1179"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1180"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1181"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1182"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1183"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1184"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1185"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1186"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1187"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1188"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1189"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1190"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1191"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1192"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1193"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1194"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1195"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1196"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1197"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1198"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1199"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1200"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1201"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1202"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1203"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1204"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1205"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1206"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1207"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1208"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1209"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1210"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1211"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1212"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1213"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1214"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1215"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1216"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1217"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1218"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1219"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1220"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1221"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1222"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1223"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1224"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1225"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1226"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1227"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1228"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1229"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1230"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1231"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1232"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>XASX</t>
   </si>
@@ -11606,9 +12516,6 @@
   </si>
   <si>
     <t>52 week low</t>
-  </si>
-  <si>
-    <t>Australian Securities Exchange</t>
   </si>
 </sst>
 </file>
@@ -13024,7 +13931,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A117B35-E7D8-6940-994B-7CCC960E3D31}" name="PivotTable7" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -13040,7 +13947,7 @@
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
-        <item x="0"/>
+        <item n="XASX" x="0"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -13124,7 +14031,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0547829C-1ED4-754B-A3EB-ED0D034B5336}" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A117B35-E7D8-6940-994B-7CCC960E3D31}" name="PivotTable6" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -13140,7 +14047,7 @@
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
-        <item x="0"/>
+        <item n="XASX" x="0"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -13429,7 +14336,7 @@
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="6">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="13">
   <a r="1" c="252">
     <v t="i">1</v>
     <v t="i">2</v>
@@ -13683,6 +14590,392 @@
     <v t="i">362</v>
     <v t="i">363</v>
     <v t="i">364</v>
+  </a>
+  <a r="1" c="252">
+    <v>1.95</v>
+    <v>1.9650000000000001</v>
+    <v>2.0099999999999998</v>
+    <v>2.0699999999999998</v>
+    <v>2.12</v>
+    <v>2.08</v>
+    <v>2.06</v>
+    <v>2.0499999999999998</v>
+    <v>2.06</v>
+    <v>2.08</v>
+    <v>2.0499999999999998</v>
+    <v>2.02</v>
+    <v>2.02</v>
+    <v>2.04</v>
+    <v>2.02</v>
+    <v>2.0099999999999998</v>
+    <v>2.02</v>
+    <v>1.9750000000000001</v>
+    <v>1.9550000000000001</v>
+    <v>2.04</v>
+    <v>1.9450000000000001</v>
+    <v>1.915</v>
+    <v>1.915</v>
+    <v>1.93</v>
+    <v>1.905</v>
+    <v>1.9650000000000001</v>
+    <v>1.9450000000000001</v>
+    <v>1.93</v>
+    <v>1.885</v>
+    <v>1.92</v>
+    <v>1.98</v>
+    <v>1.9750000000000001</v>
+    <v>2.02</v>
+    <v>2.06</v>
+    <v>2.0299999999999998</v>
+    <v>2.0299999999999998</v>
+    <v>2.04</v>
+    <v>2.02</v>
+    <v>2</v>
+    <v>1.7749999999999999</v>
+    <v>1.8149999999999999</v>
+    <v>1.8</v>
+    <v>1.85</v>
+    <v>1.9</v>
+    <v>1.86</v>
+    <v>1.89</v>
+    <v>1.905</v>
+    <v>1.9</v>
+    <v>1.905</v>
+    <v>1.88</v>
+    <v>1.865</v>
+    <v>1.925</v>
+    <v>1.9</v>
+    <v>1.89</v>
+    <v>1.93</v>
+    <v>1.98</v>
+    <v>2.04</v>
+    <v>1.9850000000000001</v>
+    <v>2.0499999999999998</v>
+    <v>2.0299999999999998</v>
+    <v>1.9950000000000001</v>
+    <v>1.97</v>
+    <v>2</v>
+    <v>2.02</v>
+    <v>2.04</v>
+    <v>2.09</v>
+    <v>2.06</v>
+    <v>2.1</v>
+    <v>2.0299999999999998</v>
+    <v>1.95</v>
+    <v>1.95</v>
+    <v>2.02</v>
+    <v>1.94</v>
+    <v>1.96</v>
+    <v>1.9550000000000001</v>
+    <v>1.98</v>
+    <v>2.02</v>
+    <v>1.95</v>
+    <v>1.97</v>
+    <v>1.9850000000000001</v>
+    <v>1.97</v>
+    <v>1.98</v>
+    <v>1.98</v>
+    <v>2.0099999999999998</v>
+    <v>2.02</v>
+    <v>1.98</v>
+    <v>2</v>
+    <v>2.0099999999999998</v>
+    <v>1.9950000000000001</v>
+    <v>1.98</v>
+    <v>1.9450000000000001</v>
+    <v>1.925</v>
+    <v>1.93</v>
+    <v>1.94</v>
+    <v>1.85</v>
+    <v>1.8</v>
+    <v>1.85</v>
+    <v>1.855</v>
+    <v>1.82</v>
+    <v>1.85</v>
+    <v>1.85</v>
+    <v>1.845</v>
+    <v>1.85</v>
+    <v>1.82</v>
+    <v>1.835</v>
+    <v>1.8049999999999999</v>
+    <v>1.8</v>
+    <v>2.25</v>
+    <v>2.38</v>
+    <v>2.38</v>
+    <v>2.4300000000000002</v>
+    <v>2.44</v>
+    <v>2.5</v>
+    <v>2.5</v>
+    <v>2.5</v>
+    <v>2.5099999999999998</v>
+    <v>2.5</v>
+    <v>2.56</v>
+    <v>2.5499999999999998</v>
+    <v>2.54</v>
+    <v>2.4900000000000002</v>
+    <v>2.5499999999999998</v>
+    <v>2.5299999999999998</v>
+    <v>2.5499999999999998</v>
+    <v>2.57</v>
+    <v>2.56</v>
+    <v>2.62</v>
+    <v>2.68</v>
+    <v>2.64</v>
+    <v>2.66</v>
+    <v>2.74</v>
+    <v>2.73</v>
+    <v>2.64</v>
+    <v>2.65</v>
+    <v>2.66</v>
+    <v>2.64</v>
+    <v>2.7</v>
+    <v>2.69</v>
+    <v>2.68</v>
+    <v>2.75</v>
+    <v>2.74</v>
+    <v>2.71</v>
+    <v>2.76</v>
+    <v>2.7</v>
+    <v>2.65</v>
+    <v>2.62</v>
+    <v>2.66</v>
+    <v>2.6</v>
+    <v>2.5499999999999998</v>
+    <v>2.5499999999999998</v>
+    <v>2.57</v>
+    <v>2.56</v>
+    <v>2.54</v>
+    <v>2.54</v>
+    <v>2.5499999999999998</v>
+    <v>2.5299999999999998</v>
+    <v>2.5499999999999998</v>
+    <v>2.54</v>
+    <v>2.56</v>
+    <v>2.6</v>
+    <v>2.56</v>
+    <v>2.61</v>
+    <v>2.59</v>
+    <v>2.52</v>
+    <v>2.4500000000000002</v>
+    <v>2.4500000000000002</v>
+    <v>2.5</v>
+    <v>2.4500000000000002</v>
+    <v>2.46</v>
+    <v>2.4500000000000002</v>
+    <v>2.36</v>
+    <v>2.2799999999999998</v>
+    <v>2.25</v>
+    <v>2.31</v>
+    <v>2.31</v>
+    <v>2.4</v>
+    <v>2.38</v>
+    <v>2.37</v>
+    <v>2.34</v>
+    <v>2.3199999999999998</v>
+    <v>2.29</v>
+    <v>2.2799999999999998</v>
+    <v>2.25</v>
+    <v>2.2799999999999998</v>
+    <v>2.29</v>
+    <v>2.39</v>
+    <v>2.4</v>
+    <v>2.25</v>
+    <v>2.37</v>
+    <v>2.4300000000000002</v>
+    <v>2.4300000000000002</v>
+    <v>2.42</v>
+    <v>2.4900000000000002</v>
+    <v>2.5099999999999998</v>
+    <v>2.48</v>
+    <v>2.5099999999999998</v>
+    <v>2.4500000000000002</v>
+    <v>2.46</v>
+    <v>2.46</v>
+    <v>2.46</v>
+    <v>2.4500000000000002</v>
+    <v>2.48</v>
+    <v>2.4300000000000002</v>
+    <v>2.4300000000000002</v>
+    <v>2.41</v>
+    <v>2.44</v>
+    <v>2.4500000000000002</v>
+    <v>2.48</v>
+    <v>2.4700000000000002</v>
+    <v>2.4900000000000002</v>
+    <v>2.4900000000000002</v>
+    <v>2.4500000000000002</v>
+    <v>2.39</v>
+    <v>2.36</v>
+    <v>2.44</v>
+    <v>2.35</v>
+    <v>2.27</v>
+    <v>2.2599999999999998</v>
+    <v>2.17</v>
+    <v>2.14</v>
+    <v>2.14</v>
+    <v>2.12</v>
+    <v>2.0699999999999998</v>
+    <v>2.1</v>
+    <v>2.16</v>
+    <v>2.13</v>
+    <v>2.09</v>
+    <v>2.11</v>
+    <v>2.1</v>
+    <v>2.15</v>
+    <v>2.17</v>
+    <v>2.13</v>
+    <v>2.11</v>
+    <v>2.11</v>
+    <v>2.08</v>
+    <v>2.04</v>
+    <v>2.11</v>
+    <v>2.1</v>
+    <v>2.1</v>
+    <v>2.0699999999999998</v>
+    <v>2.08</v>
+    <v>2.04</v>
+    <v>2.02</v>
+    <v>2.0299999999999998</v>
+    <v>2.02</v>
+    <v>1.83</v>
+    <v>1.7849999999999999</v>
+    <v>1.7849999999999999</v>
+    <v>1.76</v>
+    <v>1.7350000000000001</v>
+    <v>1.7649999999999999</v>
+    <v>1.6950000000000001</v>
+  </a>
+  <a r="1" c="20">
+    <v t="i">1</v>
+    <v t="i">2</v>
+    <v t="i">3</v>
+    <v t="i">7</v>
+    <v t="i">8</v>
+    <v t="i">9</v>
+    <v t="i">10</v>
+    <v t="i">13</v>
+    <v t="i">14</v>
+    <v t="i">15</v>
+    <v t="i">16</v>
+    <v t="i">17</v>
+    <v t="i">20</v>
+    <v t="i">21</v>
+    <v t="i">22</v>
+    <v t="i">23</v>
+    <v t="i">24</v>
+    <v t="i">27</v>
+    <v t="i">28</v>
+    <v t="i">29</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.11</v>
+    <v>2.11</v>
+    <v>2.08</v>
+    <v>2.04</v>
+    <v>2.11</v>
+    <v>2.1</v>
+    <v>2.1</v>
+    <v>2.0699999999999998</v>
+    <v>2.08</v>
+    <v>2.04</v>
+    <v>2.02</v>
+    <v>2.0299999999999998</v>
+    <v>2.02</v>
+    <v>1.83</v>
+    <v>1.7849999999999999</v>
+    <v>1.7849999999999999</v>
+    <v>1.76</v>
+    <v>1.7350000000000001</v>
+    <v>1.7649999999999999</v>
+    <v>1.6950000000000001</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.14</v>
+    <v>2.14</v>
+    <v>2.11</v>
+    <v>2.0699999999999998</v>
+    <v>2.0499999999999998</v>
+    <v>2.11</v>
+    <v>2.1</v>
+    <v>2.12</v>
+    <v>2.1</v>
+    <v>2.08</v>
+    <v>2.06</v>
+    <v>2.0299999999999998</v>
+    <v>2.0499999999999998</v>
+    <v>2.02</v>
+    <v>1.81</v>
+    <v>1.83</v>
+    <v>1.79</v>
+    <v>1.7749999999999999</v>
+    <v>1.7450000000000001</v>
+    <v>1.75</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.14</v>
+    <v>2.15</v>
+    <v>2.13</v>
+    <v>2.12</v>
+    <v>2.13</v>
+    <v>2.11</v>
+    <v>2.125</v>
+    <v>2.13</v>
+    <v>2.11</v>
+    <v>2.08</v>
+    <v>2.06</v>
+    <v>2.0499999999999998</v>
+    <v>2.06</v>
+    <v>2.1</v>
+    <v>1.82</v>
+    <v>1.845</v>
+    <v>1.81</v>
+    <v>1.78</v>
+    <v>1.77</v>
+    <v>1.75</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.1</v>
+    <v>2.1</v>
+    <v>2.08</v>
+    <v>2.0350000000000001</v>
+    <v>2.0499999999999998</v>
+    <v>2.0750000000000002</v>
+    <v>2.08</v>
+    <v>2.06</v>
+    <v>2.0499999999999998</v>
+    <v>2.04</v>
+    <v>2.02</v>
+    <v>1.9975000000000001</v>
+    <v>2.02</v>
+    <v>1.8049999999999999</v>
+    <v>1.7250000000000001</v>
+    <v>1.7649999999999999</v>
+    <v>1.7450000000000001</v>
+    <v>1.7250000000000001</v>
+    <v>1.69</v>
+    <v>1.6950000000000001</v>
+  </a>
+  <a r="1" c="20">
+    <v>163561</v>
+    <v>114420</v>
+    <v>274815</v>
+    <v>379096</v>
+    <v>458702</v>
+    <v>272035</v>
+    <v>223945</v>
+    <v>270921</v>
+    <v>363435</v>
+    <v>317437</v>
+    <v>415764</v>
+    <v>682482</v>
+    <v>638750</v>
+    <v>2052351</v>
+    <v>3501301</v>
+    <v>1482210</v>
+    <v>1705535</v>
+    <v>1347584</v>
+    <v>1689127</v>
+    <v>1336960</v>
   </a>
   <a r="1" c="252">
     <v>27.25</v>
@@ -14958,7 +16251,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1168">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1261">
   <rv s="0">
     <v>0</v>
     <v>USD/AUD</v>
@@ -14973,18 +16266,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.0500000000000001E-2</v>
-    <v>-7.4009999999999996E-3</v>
+    <v>-1.0200000000000001E-2</v>
+    <v>-7.1890000000000001E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.817430555559</v>
+    <v>44951.821018518516</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4083000000000001</v>
+    <v>1.4086000000000001</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -19923,6 +21216,370 @@
     <fb>31.34</fb>
     <v>14</v>
   </rv>
+  <rv s="6">
+    <fb>1.9650000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.0099999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.06</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.0499999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.04</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.9750000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.9450000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.915</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.905</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.98</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.0299999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7749999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.8149999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.8</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.85</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.88</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.865</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.9850000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.9950000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.1</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.835</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.8049999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.38</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.44</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.5</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.56</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.5499999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.54</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.4900000000000002</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.5299999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.57</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.62</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.68</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.64</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.66</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.73</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.69</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.71</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.76</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.6</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.61</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.59</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.52</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.46</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.36</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.2799999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.4</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.34</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.29</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.39</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.42</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.48</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.41</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.4700000000000002</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.17</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.14</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7849999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.76</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7350000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7649999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.6950000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>163561</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>114420</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>274815</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>379096</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.0350000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>458702</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>272035</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.0750000000000002</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>223945</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.125</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>270921</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>363435</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>317437</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>415764</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>682482</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.9975000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>638750</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2052351</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3501301</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7250000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1482210</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1705535</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.79</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1.7450000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1347584</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.78</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1689127</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.69</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1336960</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1.75</fb>
+    <v>14</v>
+  </rv>
   <rv s="2">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa533m&amp;q=XASX%3aBLD&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -19955,7 +21612,7 @@
     <v>Construction Materials</v>
     <v>Stock</v>
     <v>44951.333344907405</v>
-    <v>1157</v>
+    <v>1248</v>
     <v>3.45</v>
     <v>3805655000</v>
     <v>BORAL LIMITED</v>
@@ -19972,7 +21629,7 @@
     <v>1960</v>
   </rv>
   <rv s="1">
-    <v>1158</v>
+    <v>1249</v>
   </rv>
   <rv s="2">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa4om7&amp;q=XASX%3aASB&amp;form=skydnc</v>
@@ -20006,7 +21663,7 @@
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
     <v>44951.333333333336</v>
-    <v>1160</v>
+    <v>1251</v>
     <v>1.6950000000000001</v>
     <v>639709900</v>
     <v>AUSTAL LIMITED</v>
@@ -20023,10 +21680,42 @@
     <v>1987</v>
   </rv>
   <rv s="1">
-    <v>1161</v>
+    <v>1252</v>
   </rv>
   <rv s="8">
-    <v>15</v>
+    <v>16</v>
+    <v>XASX:ASB</v>
+    <v>Daily</v>
+    <v>44587</v>
+    <v>44952</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638102016000000000,638102725407651921,0</v>
+    <v>0</v>
+    <v>aa4om7</v>
+    <v>XASX:ASB</v>
+    <v>1</v>
+  </rv>
+  <rv s="9">
+    <v>17</v>
+    <v>XASX:ASB</v>
+    <v>Daily</v>
+    <v>44922</v>
+    <v>44952</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638102016000000000,638102726177351035,0</v>
+    <v>2</v>
+    <v>aa4om7</v>
+    <v>XASX:ASB</v>
+    <v>3</v>
+    <v>4</v>
+    <v>5</v>
+    <v>6</v>
+    <v>7</v>
+  </rv>
+  <rv s="8">
+    <v>16</v>
     <v>aa81zr</v>
     <v>Daily</v>
     <v>44587</v>
@@ -20037,10 +21726,10 @@
     <v>0</v>
     <v>aa81zr</v>
     <v>XASX:NAB</v>
-    <v>1</v>
+    <v>8</v>
   </rv>
   <rv s="8">
-    <v>15</v>
+    <v>16</v>
     <v>aa5cec</v>
     <v>Daily</v>
     <v>44587</v>
@@ -20051,10 +21740,10 @@
     <v>0</v>
     <v>aa5cec</v>
     <v>XASX:CBA</v>
-    <v>2</v>
+    <v>9</v>
   </rv>
   <rv s="8">
-    <v>15</v>
+    <v>16</v>
     <v>aa4pa2</v>
     <v>Daily</v>
     <v>44587</v>
@@ -20065,10 +21754,10 @@
     <v>0</v>
     <v>aa4pa2</v>
     <v>XASX:ASX</v>
-    <v>3</v>
+    <v>10</v>
   </rv>
   <rv s="8">
-    <v>15</v>
+    <v>16</v>
     <v>aa5c2w</v>
     <v>Daily</v>
     <v>44587</v>
@@ -20079,10 +21768,10 @@
     <v>0</v>
     <v>aa5c2w</v>
     <v>XASX:CAT</v>
-    <v>4</v>
+    <v>11</v>
   </rv>
   <rv s="8">
-    <v>15</v>
+    <v>16</v>
     <v>aa658m</v>
     <v>Daily</v>
     <v>44587</v>
@@ -20093,13 +21782,13 @@
     <v>0</v>
     <v>aa658m</v>
     <v>XASX:EOS</v>
-    <v>5</v>
+    <v>12</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="10">
   <s t="_linkedentitycore">
     <k n="_Display" t="spb"/>
     <k n="_DisplayString" t="s"/>
@@ -20288,6 +21977,24 @@
     <k n="Instrument" t="s"/>
     <k n="Close" t="a"/>
   </s>
+  <s t="_stockhistorycache">
+    <k n="_Format" t="spb"/>
+    <k n="Symbol" t="s"/>
+    <k n="Interval" t="s"/>
+    <k n="StartDate" t="i"/>
+    <k n="EndDate" t="i"/>
+    <k n="f1904" t="b"/>
+    <k n="fdcompat" t="b"/>
+    <k n="etag" t="s"/>
+    <k n="Date" t="a"/>
+    <k n="EntityId" t="s"/>
+    <k n="Instrument" t="s"/>
+    <k n="Close" t="a"/>
+    <k n="Open" t="a"/>
+    <k n="High" t="a"/>
+    <k n="Low" t="a"/>
+    <k n="Volume" t="a"/>
+  </s>
 </rvStructures>
 </file>
 
@@ -20455,7 +22162,7 @@
       <v t="s">%OutdatedReason</v>
     </a>
   </spbArrays>
-  <spbData count="16">
+  <spbData count="18">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -20583,16 +22290,27 @@
     <spb s="11">
       <v>1</v>
     </spb>
+    <spb s="11">
+      <v>7</v>
+    </spb>
     <spb s="12">
       <v>12</v>
       <v>1</v>
+    </spb>
+    <spb s="13">
+      <v>1</v>
+      <v>12</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>7</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="13">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="14">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -20710,6 +22428,14 @@
   <s>
     <k n="Date" t="i"/>
     <k n="Close" t="i"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="Date" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Close" t="i"/>
+    <k n="Volume" t="i"/>
   </s>
 </spbStructures>
 </file>
@@ -21196,7 +22922,7 @@
       </c>
       <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4083▼</v>
+        <v>$1.4086▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -28353,20 +30079,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A53158-39AD-6F4A-9FB2-AE17C2A023A7}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65173A22-D60C-684F-AC10-940F91797BDE}">
+  <dimension ref="A1:IT26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -28374,7 +30099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -28382,12 +30107,1566 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
+      </c>
+      <c r="C4" cm="1" vm="894">
+        <f t="array" aca="1" ref="C4:IT4" ca="1">TRANSPOSE(_xlfn.STOCKHISTORY(A4&amp;":"&amp;B4, TODAY()-365, TODAY(),0,0,1))</f>
+        <v>1.95</v>
+      </c>
+      <c r="D4" vm="1141">
+        <f ca="1"/>
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="E4" vm="1142">
+        <f ca="1"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F4" vm="888">
+        <f ca="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G4" vm="887">
+        <f ca="1"/>
+        <v>2.12</v>
+      </c>
+      <c r="H4" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="I4" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="J4" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K4" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="L4" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="M4" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="N4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="O4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="P4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="Q4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="R4" vm="1142">
+        <f ca="1"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="S4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="T4" vm="1146">
+        <f ca="1"/>
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="U4" vm="893">
+        <f ca="1"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="V4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="W4" vm="1147">
+        <f ca="1"/>
+        <v>1.9450000000000001</v>
+      </c>
+      <c r="X4" vm="1148">
+        <f ca="1"/>
+        <v>1.915</v>
+      </c>
+      <c r="Y4" vm="1148">
+        <f ca="1"/>
+        <v>1.915</v>
+      </c>
+      <c r="Z4" vm="895">
+        <f ca="1"/>
+        <v>1.93</v>
+      </c>
+      <c r="AA4" vm="1149">
+        <f ca="1"/>
+        <v>1.905</v>
+      </c>
+      <c r="AB4" vm="1141">
+        <f ca="1"/>
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="AC4" vm="1147">
+        <f ca="1"/>
+        <v>1.9450000000000001</v>
+      </c>
+      <c r="AD4" vm="895">
+        <f ca="1"/>
+        <v>1.93</v>
+      </c>
+      <c r="AE4" vm="853">
+        <f ca="1"/>
+        <v>1.885</v>
+      </c>
+      <c r="AF4" vm="861">
+        <f ca="1"/>
+        <v>1.92</v>
+      </c>
+      <c r="AG4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="AH4" vm="1146">
+        <f ca="1"/>
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="AI4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="AJ4" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="AK4" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AL4" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AM4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="AN4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="AO4" vm="848">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="AP4" vm="1152">
+        <f ca="1"/>
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="AQ4" vm="1153">
+        <f ca="1"/>
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="AR4" vm="1154">
+        <f ca="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="AS4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="AT4" vm="896">
+        <f ca="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="AU4" vm="835">
+        <f ca="1"/>
+        <v>1.86</v>
+      </c>
+      <c r="AV4" vm="849">
+        <f ca="1"/>
+        <v>1.89</v>
+      </c>
+      <c r="AW4" vm="1149">
+        <f ca="1"/>
+        <v>1.905</v>
+      </c>
+      <c r="AX4" vm="896">
+        <f ca="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="AY4" vm="1149">
+        <f ca="1"/>
+        <v>1.905</v>
+      </c>
+      <c r="AZ4" vm="1156">
+        <f ca="1"/>
+        <v>1.88</v>
+      </c>
+      <c r="BA4" vm="1157">
+        <f ca="1"/>
+        <v>1.865</v>
+      </c>
+      <c r="BB4" vm="890">
+        <f ca="1"/>
+        <v>1.925</v>
+      </c>
+      <c r="BC4" vm="896">
+        <f ca="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="BD4" vm="849">
+        <f ca="1"/>
+        <v>1.89</v>
+      </c>
+      <c r="BE4" vm="895">
+        <f ca="1"/>
+        <v>1.93</v>
+      </c>
+      <c r="BF4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="BG4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="BH4" vm="1158">
+        <f ca="1"/>
+        <v>1.9850000000000001</v>
+      </c>
+      <c r="BI4" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BJ4" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BK4" vm="1159">
+        <f ca="1"/>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="BL4" vm="850">
+        <f ca="1"/>
+        <v>1.97</v>
+      </c>
+      <c r="BM4" vm="848">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="BN4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="BO4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="BP4" vm="885">
+        <f ca="1"/>
+        <v>2.09</v>
+      </c>
+      <c r="BQ4" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="BR4" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="BS4" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BT4" vm="894">
+        <f ca="1"/>
+        <v>1.95</v>
+      </c>
+      <c r="BU4" vm="894">
+        <f ca="1"/>
+        <v>1.95</v>
+      </c>
+      <c r="BV4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="BW4" vm="860">
+        <f ca="1"/>
+        <v>1.94</v>
+      </c>
+      <c r="BX4" vm="892">
+        <f ca="1"/>
+        <v>1.96</v>
+      </c>
+      <c r="BY4" vm="893">
+        <f ca="1"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="BZ4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="CA4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="CB4" vm="894">
+        <f ca="1"/>
+        <v>1.95</v>
+      </c>
+      <c r="CC4" vm="850">
+        <f ca="1"/>
+        <v>1.97</v>
+      </c>
+      <c r="CD4" vm="1158">
+        <f ca="1"/>
+        <v>1.9850000000000001</v>
+      </c>
+      <c r="CE4" vm="850">
+        <f ca="1"/>
+        <v>1.97</v>
+      </c>
+      <c r="CF4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="CG4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="CH4" vm="1142">
+        <f ca="1"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="CI4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="CJ4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="CK4" vm="848">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="CL4" vm="1142">
+        <f ca="1"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="CM4" vm="1159">
+        <f ca="1"/>
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="CN4" vm="1150">
+        <f ca="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="CO4" vm="1147">
+        <f ca="1"/>
+        <v>1.9450000000000001</v>
+      </c>
+      <c r="CP4" vm="890">
+        <f ca="1"/>
+        <v>1.925</v>
+      </c>
+      <c r="CQ4" vm="895">
+        <f ca="1"/>
+        <v>1.93</v>
+      </c>
+      <c r="CR4" vm="860">
+        <f ca="1"/>
+        <v>1.94</v>
+      </c>
+      <c r="CS4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="CT4" vm="1154">
+        <f ca="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="CU4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="CV4" vm="851">
+        <f ca="1"/>
+        <v>1.855</v>
+      </c>
+      <c r="CW4" vm="854">
+        <f ca="1"/>
+        <v>1.82</v>
+      </c>
+      <c r="CX4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="CY4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="CZ4" vm="898">
+        <f ca="1"/>
+        <v>1.845</v>
+      </c>
+      <c r="DA4" vm="1155">
+        <f ca="1"/>
+        <v>1.85</v>
+      </c>
+      <c r="DB4" vm="854">
+        <f ca="1"/>
+        <v>1.82</v>
+      </c>
+      <c r="DC4" vm="1161">
+        <f ca="1"/>
+        <v>1.835</v>
+      </c>
+      <c r="DD4" vm="1162">
+        <f ca="1"/>
+        <v>1.8049999999999999</v>
+      </c>
+      <c r="DE4" vm="1154">
+        <f ca="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="DF4" vm="882">
+        <f ca="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="DG4" vm="1163">
+        <f ca="1"/>
+        <v>2.38</v>
+      </c>
+      <c r="DH4" vm="1163">
+        <f ca="1"/>
+        <v>2.38</v>
+      </c>
+      <c r="DI4" vm="880">
+        <f ca="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="DJ4" vm="1164">
+        <f ca="1"/>
+        <v>2.44</v>
+      </c>
+      <c r="DK4" vm="1165">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="DL4" vm="1165">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="DM4" vm="1165">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="DN4" vm="863">
+        <f ca="1"/>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="DO4" vm="1165">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="DP4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="DQ4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="DR4" vm="1168">
+        <f ca="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="DS4" vm="1169">
+        <f ca="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="DT4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="DU4" vm="1170">
+        <f ca="1"/>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="DV4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="DW4" vm="1171">
+        <f ca="1"/>
+        <v>2.57</v>
+      </c>
+      <c r="DX4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="DY4" vm="1172">
+        <f ca="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="DZ4" vm="1173">
+        <f ca="1"/>
+        <v>2.68</v>
+      </c>
+      <c r="EA4" vm="1174">
+        <f ca="1"/>
+        <v>2.64</v>
+      </c>
+      <c r="EB4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="EC4" vm="875">
+        <f ca="1"/>
+        <v>2.74</v>
+      </c>
+      <c r="ED4" vm="1176">
+        <f ca="1"/>
+        <v>2.73</v>
+      </c>
+      <c r="EE4" vm="1174">
+        <f ca="1"/>
+        <v>2.64</v>
+      </c>
+      <c r="EF4" vm="878">
+        <f ca="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="EG4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="EH4" vm="1174">
+        <f ca="1"/>
+        <v>2.64</v>
+      </c>
+      <c r="EI4" vm="874">
+        <f ca="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="EJ4" vm="1177">
+        <f ca="1"/>
+        <v>2.69</v>
+      </c>
+      <c r="EK4" vm="1173">
+        <f ca="1"/>
+        <v>2.68</v>
+      </c>
+      <c r="EL4" vm="870">
+        <f ca="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="EM4" vm="875">
+        <f ca="1"/>
+        <v>2.74</v>
+      </c>
+      <c r="EN4" vm="1178">
+        <f ca="1"/>
+        <v>2.71</v>
+      </c>
+      <c r="EO4" vm="1179">
+        <f ca="1"/>
+        <v>2.76</v>
+      </c>
+      <c r="EP4" vm="874">
+        <f ca="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="EQ4" vm="878">
+        <f ca="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="ER4" vm="1172">
+        <f ca="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="ES4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="ET4" vm="1180">
+        <f ca="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="EU4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="EV4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="EW4" vm="1171">
+        <f ca="1"/>
+        <v>2.57</v>
+      </c>
+      <c r="EX4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="EY4" vm="1168">
+        <f ca="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="EZ4" vm="1168">
+        <f ca="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="FA4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="FB4" vm="1170">
+        <f ca="1"/>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="FC4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="FD4" vm="1168">
+        <f ca="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="FE4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="FF4" vm="1180">
+        <f ca="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="FG4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="FH4" vm="1181">
+        <f ca="1"/>
+        <v>2.61</v>
+      </c>
+      <c r="FI4" vm="1182">
+        <f ca="1"/>
+        <v>2.59</v>
+      </c>
+      <c r="FJ4" vm="1183">
+        <f ca="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="FK4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="FL4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="FM4" vm="1165">
+        <f ca="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="FN4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="FO4" vm="1184">
+        <f ca="1"/>
+        <v>2.46</v>
+      </c>
+      <c r="FP4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="FQ4" vm="1185">
+        <f ca="1"/>
+        <v>2.36</v>
+      </c>
+      <c r="FR4" vm="1186">
+        <f ca="1"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="FS4" vm="882">
+        <f ca="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="FT4" vm="838">
+        <f ca="1"/>
+        <v>2.31</v>
+      </c>
+      <c r="FU4" vm="838">
+        <f ca="1"/>
+        <v>2.31</v>
+      </c>
+      <c r="FV4" vm="1187">
+        <f ca="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="FW4" vm="1163">
+        <f ca="1"/>
+        <v>2.38</v>
+      </c>
+      <c r="FX4" vm="881">
+        <f ca="1"/>
+        <v>2.37</v>
+      </c>
+      <c r="FY4" vm="1188">
+        <f ca="1"/>
+        <v>2.34</v>
+      </c>
+      <c r="FZ4" vm="883">
+        <f ca="1"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="GA4" vm="1189">
+        <f ca="1"/>
+        <v>2.29</v>
+      </c>
+      <c r="GB4" vm="1186">
+        <f ca="1"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="GC4" vm="882">
+        <f ca="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="GD4" vm="1186">
+        <f ca="1"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="GE4" vm="1189">
+        <f ca="1"/>
+        <v>2.29</v>
+      </c>
+      <c r="GF4" vm="1190">
+        <f ca="1"/>
+        <v>2.39</v>
+      </c>
+      <c r="GG4" vm="1187">
+        <f ca="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="GH4" vm="882">
+        <f ca="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="GI4" vm="881">
+        <f ca="1"/>
+        <v>2.37</v>
+      </c>
+      <c r="GJ4" vm="880">
+        <f ca="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="GK4" vm="880">
+        <f ca="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="GL4" vm="1191">
+        <f ca="1"/>
+        <v>2.42</v>
+      </c>
+      <c r="GM4" vm="1169">
+        <f ca="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="GN4" vm="863">
+        <f ca="1"/>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="GO4" vm="1192">
+        <f ca="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="GP4" vm="863">
+        <f ca="1"/>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="GQ4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="GR4" vm="1184">
+        <f ca="1"/>
+        <v>2.46</v>
+      </c>
+      <c r="GS4" vm="1184">
+        <f ca="1"/>
+        <v>2.46</v>
+      </c>
+      <c r="GT4" vm="1184">
+        <f ca="1"/>
+        <v>2.46</v>
+      </c>
+      <c r="GU4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="GV4" vm="1192">
+        <f ca="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="GW4" vm="880">
+        <f ca="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="GX4" vm="880">
+        <f ca="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="GY4" vm="1193">
+        <f ca="1"/>
+        <v>2.41</v>
+      </c>
+      <c r="GZ4" vm="1164">
+        <f ca="1"/>
+        <v>2.44</v>
+      </c>
+      <c r="HA4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="HB4" vm="1192">
+        <f ca="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="HC4" vm="1194">
+        <f ca="1"/>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="HD4" vm="1169">
+        <f ca="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="HE4" vm="1169">
+        <f ca="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="HF4" vm="879">
+        <f ca="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="HG4" vm="1190">
+        <f ca="1"/>
+        <v>2.39</v>
+      </c>
+      <c r="HH4" vm="1185">
+        <f ca="1"/>
+        <v>2.36</v>
+      </c>
+      <c r="HI4" vm="1164">
+        <f ca="1"/>
+        <v>2.44</v>
+      </c>
+      <c r="HJ4" vm="862">
+        <f ca="1"/>
+        <v>2.35</v>
+      </c>
+      <c r="HK4" vm="844">
+        <f ca="1"/>
+        <v>2.27</v>
+      </c>
+      <c r="HL4" vm="841">
+        <f ca="1"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="HM4" vm="1195">
+        <f ca="1"/>
+        <v>2.17</v>
+      </c>
+      <c r="HN4" vm="1196">
+        <f ca="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="HO4" vm="1196">
+        <f ca="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="HP4" vm="887">
+        <f ca="1"/>
+        <v>2.12</v>
+      </c>
+      <c r="HQ4" vm="888">
+        <f ca="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="HR4" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="HS4" vm="837">
+        <f ca="1"/>
+        <v>2.16</v>
+      </c>
+      <c r="HT4" vm="846">
+        <f ca="1"/>
+        <v>2.13</v>
+      </c>
+      <c r="HU4" vm="885">
+        <f ca="1"/>
+        <v>2.09</v>
+      </c>
+      <c r="HV4" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="HW4" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="HX4" vm="842">
+        <f ca="1"/>
+        <v>2.15</v>
+      </c>
+      <c r="HY4" vm="1195">
+        <f ca="1"/>
+        <v>2.17</v>
+      </c>
+      <c r="HZ4" vm="846">
+        <f ca="1"/>
+        <v>2.13</v>
+      </c>
+      <c r="IA4" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="IB4" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="IC4" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="ID4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="IE4" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="IF4" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="IG4" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="IH4" vm="888">
+        <f ca="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="II4" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="IJ4" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="IK4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="IL4" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="IM4" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="IN4" vm="834">
+        <f ca="1"/>
+        <v>1.83</v>
+      </c>
+      <c r="IO4" vm="1197">
+        <f ca="1"/>
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="IP4" vm="1197">
+        <f ca="1"/>
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="IQ4" vm="1198">
+        <f ca="1"/>
+        <v>1.76</v>
+      </c>
+      <c r="IR4" vm="1199">
+        <f ca="1"/>
+        <v>1.7350000000000001</v>
+      </c>
+      <c r="IS4" vm="1200">
+        <f ca="1"/>
+        <v>1.7649999999999999</v>
+      </c>
+      <c r="IT4" vm="1201">
+        <f ca="1"/>
+        <v>1.6950000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A6" t="str" cm="1">
+        <f t="array" aca="1" ref="A6:F26" ca="1">(_xlfn.STOCKHISTORY(A4&amp;":"&amp;B4, TODAY()-30, TODAY(),0,1,0,5,2,3,4,1))</f>
+        <v>Date</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1"/>
+        <v>Volume</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1"/>
+        <v>Open</v>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1"/>
+        <v>High</v>
+      </c>
+      <c r="E6" t="str">
+        <f ca="1"/>
+        <v>Low</v>
+      </c>
+      <c r="F6" t="str">
+        <f ca="1"/>
+        <v>Close</v>
+      </c>
+    </row>
+    <row r="7" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A7" vm="242">
+        <f ca="1"/>
+        <v>44923</v>
+      </c>
+      <c r="B7" vm="1202">
+        <f ca="1"/>
+        <v>163561</v>
+      </c>
+      <c r="C7" vm="1196">
+        <f ca="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="D7" vm="1196">
+        <f ca="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="E7" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="F7" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A8" vm="243">
+        <f ca="1"/>
+        <v>44924</v>
+      </c>
+      <c r="B8" vm="1203">
+        <f ca="1"/>
+        <v>114420</v>
+      </c>
+      <c r="C8" vm="1196">
+        <f ca="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="D8" vm="842">
+        <f ca="1"/>
+        <v>2.15</v>
+      </c>
+      <c r="E8" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="F8" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A9" vm="244">
+        <f ca="1"/>
+        <v>44925</v>
+      </c>
+      <c r="B9" vm="1204">
+        <f ca="1"/>
+        <v>274815</v>
+      </c>
+      <c r="C9" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="D9" vm="846">
+        <f ca="1"/>
+        <v>2.13</v>
+      </c>
+      <c r="E9" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="F9" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A10" vm="245">
+        <f ca="1"/>
+        <v>44929</v>
+      </c>
+      <c r="B10" vm="1205">
+        <f ca="1"/>
+        <v>379096</v>
+      </c>
+      <c r="C10" vm="888">
+        <f ca="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="D10" vm="887">
+        <f ca="1"/>
+        <v>2.12</v>
+      </c>
+      <c r="E10" vm="1206">
+        <f ca="1"/>
+        <v>2.0350000000000001</v>
+      </c>
+      <c r="F10" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A11" vm="246">
+        <f ca="1"/>
+        <v>44930</v>
+      </c>
+      <c r="B11" vm="1207">
+        <f ca="1"/>
+        <v>458702</v>
+      </c>
+      <c r="C11" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D11" vm="846">
+        <f ca="1"/>
+        <v>2.13</v>
+      </c>
+      <c r="E11" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F11" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A12" vm="247">
+        <f ca="1"/>
+        <v>44931</v>
+      </c>
+      <c r="B12" vm="1208">
+        <f ca="1"/>
+        <v>272035</v>
+      </c>
+      <c r="C12" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="D12" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="E12" vm="1209">
+        <f ca="1"/>
+        <v>2.0750000000000002</v>
+      </c>
+      <c r="F12" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A13" vm="248">
+        <f ca="1"/>
+        <v>44932</v>
+      </c>
+      <c r="B13" vm="1210">
+        <f ca="1"/>
+        <v>223945</v>
+      </c>
+      <c r="C13" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="D13" vm="1211">
+        <f ca="1"/>
+        <v>2.125</v>
+      </c>
+      <c r="E13" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="F13" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A14" vm="249">
+        <f ca="1"/>
+        <v>44935</v>
+      </c>
+      <c r="B14" vm="1212">
+        <f ca="1"/>
+        <v>270921</v>
+      </c>
+      <c r="C14" vm="887">
+        <f ca="1"/>
+        <v>2.12</v>
+      </c>
+      <c r="D14" vm="846">
+        <f ca="1"/>
+        <v>2.13</v>
+      </c>
+      <c r="E14" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="F14" vm="888">
+        <f ca="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A15" vm="250">
+        <f ca="1"/>
+        <v>44936</v>
+      </c>
+      <c r="B15" vm="1213">
+        <f ca="1"/>
+        <v>363435</v>
+      </c>
+      <c r="C15" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="D15" vm="845">
+        <f ca="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="E15" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F15" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A16" vm="251">
+        <f ca="1"/>
+        <v>44937</v>
+      </c>
+      <c r="B16" vm="1214">
+        <f ca="1"/>
+        <v>317437</v>
+      </c>
+      <c r="C16" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="D16" vm="836">
+        <f ca="1"/>
+        <v>2.08</v>
+      </c>
+      <c r="E16" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="F16" vm="1145">
+        <f ca="1"/>
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" vm="252">
+        <f ca="1"/>
+        <v>44938</v>
+      </c>
+      <c r="B17" vm="1215">
+        <f ca="1"/>
+        <v>415764</v>
+      </c>
+      <c r="C17" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="D17" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="E17" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="F17" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" vm="253">
+        <f ca="1"/>
+        <v>44939</v>
+      </c>
+      <c r="B18" vm="1216">
+        <f ca="1"/>
+        <v>682482</v>
+      </c>
+      <c r="C18" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D18" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E18" vm="1217">
+        <f ca="1"/>
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="F18" vm="1151">
+        <f ca="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" vm="254">
+        <f ca="1"/>
+        <v>44942</v>
+      </c>
+      <c r="B19" vm="1218">
+        <f ca="1"/>
+        <v>638750</v>
+      </c>
+      <c r="C19" vm="1144">
+        <f ca="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D19" vm="1143">
+        <f ca="1"/>
+        <v>2.06</v>
+      </c>
+      <c r="E19" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="F19" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" vm="255">
+        <f ca="1"/>
+        <v>44943</v>
+      </c>
+      <c r="B20" vm="1219">
+        <f ca="1"/>
+        <v>2052351</v>
+      </c>
+      <c r="C20" vm="889">
+        <f ca="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="D20" vm="1160">
+        <f ca="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="E20" vm="1162">
+        <f ca="1"/>
+        <v>1.8049999999999999</v>
+      </c>
+      <c r="F20" vm="834">
+        <f ca="1"/>
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" vm="256">
+        <f ca="1"/>
+        <v>44944</v>
+      </c>
+      <c r="B21" vm="1220">
+        <f ca="1"/>
+        <v>3501301</v>
+      </c>
+      <c r="C21" vm="859">
+        <f ca="1"/>
+        <v>1.81</v>
+      </c>
+      <c r="D21" vm="854">
+        <f ca="1"/>
+        <v>1.82</v>
+      </c>
+      <c r="E21" vm="1221">
+        <f ca="1"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="F21" vm="1197">
+        <f ca="1"/>
+        <v>1.7849999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" vm="257">
+        <f ca="1"/>
+        <v>44945</v>
+      </c>
+      <c r="B22" vm="1222">
+        <f ca="1"/>
+        <v>1482210</v>
+      </c>
+      <c r="C22" vm="834">
+        <f ca="1"/>
+        <v>1.83</v>
+      </c>
+      <c r="D22" vm="898">
+        <f ca="1"/>
+        <v>1.845</v>
+      </c>
+      <c r="E22" vm="1200">
+        <f ca="1"/>
+        <v>1.7649999999999999</v>
+      </c>
+      <c r="F22" vm="1197">
+        <f ca="1"/>
+        <v>1.7849999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" vm="258">
+        <f ca="1"/>
+        <v>44946</v>
+      </c>
+      <c r="B23" vm="1223">
+        <f ca="1"/>
+        <v>1705535</v>
+      </c>
+      <c r="C23" vm="1224">
+        <f ca="1"/>
+        <v>1.79</v>
+      </c>
+      <c r="D23" vm="859">
+        <f ca="1"/>
+        <v>1.81</v>
+      </c>
+      <c r="E23" vm="1225">
+        <f ca="1"/>
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="F23" vm="1198">
+        <f ca="1"/>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" vm="259">
+        <f ca="1"/>
+        <v>44949</v>
+      </c>
+      <c r="B24" vm="1226">
+        <f ca="1"/>
+        <v>1347584</v>
+      </c>
+      <c r="C24" vm="1152">
+        <f ca="1"/>
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="D24" vm="1227">
+        <f ca="1"/>
+        <v>1.78</v>
+      </c>
+      <c r="E24" vm="1221">
+        <f ca="1"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="F24" vm="1199">
+        <f ca="1"/>
+        <v>1.7350000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" vm="260">
+        <f ca="1"/>
+        <v>44950</v>
+      </c>
+      <c r="B25" vm="1228">
+        <f ca="1"/>
+        <v>1689127</v>
+      </c>
+      <c r="C25" vm="1225">
+        <f ca="1"/>
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="D25" vm="855">
+        <f ca="1"/>
+        <v>1.77</v>
+      </c>
+      <c r="E25" vm="1229">
+        <f ca="1"/>
+        <v>1.69</v>
+      </c>
+      <c r="F25" vm="1200">
+        <f ca="1"/>
+        <v>1.7649999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" vm="261">
+        <f ca="1"/>
+        <v>44951</v>
+      </c>
+      <c r="B26" vm="1230">
+        <f ca="1"/>
+        <v>1336960</v>
+      </c>
+      <c r="C26" vm="1231">
+        <f ca="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="D26" vm="1231">
+        <f ca="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="E26" vm="1201">
+        <f ca="1"/>
+        <v>1.6950000000000001</v>
+      </c>
+      <c r="F26" vm="1201">
+        <f ca="1"/>
+        <v>1.6950000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -28396,19 +31675,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33D8CFE-9DEC-4C44-9F11-E2A67B5A6207}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38F13E4-FF82-6E40-B343-A0462498EE32}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -28416,7 +31693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -28424,16 +31701,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="e" cm="1">
-        <f t="array" aca="1" ref="C4" ca="1">TRANSPOSE(_xlfn.STOCKHISTORY(A4&amp;":"&amp;B4, TODAY()-365, TODAY, 0,0,1))</f>
-        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -28445,8 +31718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B519C-9D84-EF42-9037-F33B25BAF358}">
   <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28485,7 +31758,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="e" vm="1141">
+      <c r="A3" t="e" vm="1232">
         <v>#VALUE!</v>
       </c>
       <c r="B3" t="str" cm="1">
@@ -28518,7 +31791,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="e" vm="1142">
+      <c r="A4" t="e" vm="1233">
         <v>#VALUE!</v>
       </c>
       <c r="B4" t="str" cm="1">

</xml_diff>

<commit_message>
Added stock chart for ASB
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595BBE5F-03D0-8F46-B19D-B09C9BC35304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2DA4D7-3A75-6645-9EE0-FDE9A8448596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7980" windowWidth="30240" windowHeight="17420" activeTab="3" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -13257,11 +13257,1297 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>ASB!$B$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>AUSTAL LIMITED (XASX:ASB)</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ASB!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Volume</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ASB!$A$7:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$B$7:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>163561</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114420</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>274815</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>379096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>458702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>272035</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>223945</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>270921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>363435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>317437</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>415764</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>682482</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>638750</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2052351</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3501301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1482210</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1705535</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1347584</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1689127</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1336960</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FDD0-7446-9495-3C5AF2FEAFAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1710978656"/>
+        <c:axId val="1710980304"/>
+      </c:barChart>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ASB!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ASB!$A$7:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$C$7:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FDD0-7446-9495-3C5AF2FEAFAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ASB!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ASB!$A$7:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$D$7:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.845</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.78</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FDD0-7446-9495-3C5AF2FEAFAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ASB!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ASB!$A$7:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$E$7:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9975000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.7649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6950000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FDD0-7446-9495-3C5AF2FEAFAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ASB!$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Close</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ASB!$A$7:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$F$7:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.7849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6950000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FDD0-7446-9495-3C5AF2FEAFAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
+        <c:axId val="1089863008"/>
+        <c:axId val="1057680704"/>
+      </c:stockChart>
+      <c:dateAx>
+        <c:axId val="1710978656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-3600000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1710980304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1710980304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0,,&quot;M&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1710978656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1057680704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1089863008"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dateAx>
+        <c:axId val="1089863008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1057680704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -13813,6 +15099,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -13846,6 +15648,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>103908</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>34635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>196272</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43688443-90C6-D849-BC9C-CD88B9E93277}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -16266,18 +18106,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.0200000000000001E-2</v>
-    <v>-7.1890000000000001E-3</v>
+    <v>-1.0699999999999999E-2</v>
+    <v>-7.5420000000000001E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.821018518516</v>
+    <v>44951.824664351851</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4086000000000001</v>
+    <v>1.4080999999999999</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -22858,8 +24698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22922,7 +24762,7 @@
       </c>
       <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4086▼</v>
+        <v>$1.4081▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -30082,8 +31922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65173A22-D60C-684F-AC10-940F91797BDE}">
   <dimension ref="A1:IT26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added last 12 months chart for asb
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2DA4D7-3A75-6645-9EE0-FDE9A8448596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43710C2-DA6B-F441-A4CC-224882670539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="-320" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -13296,14 +13296,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -14503,6 +14503,1015 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200">
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Close Last 12 Months</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>ASB!$C$4:$IT$4</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="252"/>
+                <c:pt idx="0">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.915</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.915</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.905</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.885</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.9750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.7749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.8149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.905</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.905</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.865</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.925</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.9850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.9550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.9850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.9950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.9450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.925</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.855</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.845</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.835</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.8049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2.34</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2.27</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2.15</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1.7849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1.7849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1.7350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1.7649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1.6950000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3133-2F48-A520-192B53A83395}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1678068351"/>
+        <c:axId val="1678174687"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1678068351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1678174687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1678174687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1678068351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -14541,6 +15550,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -15615,6 +16664,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15627,8 +17197,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>191507</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15686,6 +17256,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>103908</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>46182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34ECC975-9BDE-474A-932C-1836087B6E02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15771,7 +17379,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A117B35-E7D8-6940-994B-7CCC960E3D31}" name="PivotTable7" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A117B35-E7D8-6940-994B-7CCC960E3D31}" name="PivotTable7" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -18106,18 +19714,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.0699999999999999E-2</v>
-    <v>-7.5420000000000001E-3</v>
+    <v>-1.11E-2</v>
+    <v>-7.8239999999999994E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.824664351851</v>
+    <v>44951.831678240742</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4080999999999999</v>
+    <v>1.4077</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -24698,7 +26306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -24762,7 +26370,7 @@
       </c>
       <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4081▼</v>
+        <v>$1.4077▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -31922,8 +33530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65173A22-D60C-684F-AC10-940F91797BDE}">
   <dimension ref="A1:IT26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="DX1" workbookViewId="0">
+      <selection activeCell="HF23" sqref="HF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added stockhistory for BLD
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43710C2-DA6B-F441-A4CC-224882670539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EB2681-BB1B-D84A-AF4C-B3B27D36CAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="-320" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="4" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -59,7 +59,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1233">
+  <futureMetadata name="XLRICHVALUE" count="1344">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -8680,6 +8680,20 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1248"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1249"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1250"/>
         </ext>
       </extLst>
@@ -8687,7 +8701,770 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1251"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1252"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1253"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1254"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1255"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1256"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1257"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1258"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1259"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1260"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1261"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1262"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1263"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1264"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1265"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1266"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1267"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1268"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1269"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1270"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1271"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1272"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1273"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1274"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1275"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1276"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1277"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1278"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1279"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1280"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1281"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1282"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1283"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1284"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1285"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1286"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1287"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1288"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1289"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1290"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1291"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1292"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1293"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1294"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1295"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1296"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1297"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1298"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1299"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1300"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1301"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1302"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1303"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1304"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1305"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1306"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1307"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1308"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1309"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1310"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1311"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1312"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1313"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1314"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1315"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1316"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1317"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1318"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1319"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1320"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1321"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1322"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1323"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1324"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1325"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1326"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1327"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1328"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1329"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1330"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1331"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1332"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1333"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1334"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1335"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1336"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1337"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1338"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1339"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1340"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1341"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1342"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1343"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1344"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1345"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1346"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1347"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1348"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1349"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1350"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1351"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1352"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1353"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1354"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1355"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1356"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1357"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1358"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1361"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1364"/>
         </ext>
       </extLst>
     </bk>
@@ -8697,7 +9474,7 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1233">
+  <valueMetadata count="1344">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -12396,6 +13173,339 @@
     </bk>
     <bk>
       <rc t="2" v="1232"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1233"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1234"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1235"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1236"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1237"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1238"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1239"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1240"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1241"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1242"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1243"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1244"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1245"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1246"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1247"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1248"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1249"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1250"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1251"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1252"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1253"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1254"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1255"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1256"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1257"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1258"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1259"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1260"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1261"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1262"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1263"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1264"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1265"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1266"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1267"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1268"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1269"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1270"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1271"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1272"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1273"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1274"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1275"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1276"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1277"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1278"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1279"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1280"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1281"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1282"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1283"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1284"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1285"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1286"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1287"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1288"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1289"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1290"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1291"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1292"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1293"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1294"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1295"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1296"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1297"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1298"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1299"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1300"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1301"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1302"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1303"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1304"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1305"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1306"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1307"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1308"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1309"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1310"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1311"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1312"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1313"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1314"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1315"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1316"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1317"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1318"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1319"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1320"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1321"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1322"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1323"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1324"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1325"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1326"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1327"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1328"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1329"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1330"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1331"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1332"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1333"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1334"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1335"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1336"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1337"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1338"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1339"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1340"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1341"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1342"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1343"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -17784,7 +18894,7 @@
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="13">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="19">
   <a r="1" c="252">
     <v t="i">1</v>
     <v t="i">2</v>
@@ -19695,11 +20805,375 @@
     <v>0.69</v>
     <v>0.67</v>
   </a>
+  <a r="1" c="252">
+    <v>5.68</v>
+    <v>5.95</v>
+    <v>5.87</v>
+    <v>6.21</v>
+    <v>6.45</v>
+    <v>6.53</v>
+    <v>3.8</v>
+    <v>3.87</v>
+    <v>3.95</v>
+    <v>3.99</v>
+    <v>3.93</v>
+    <v>3.79</v>
+    <v>3.72</v>
+    <v>3.63</v>
+    <v>3.71</v>
+    <v>3.73</v>
+    <v>3.71</v>
+    <v>3.71</v>
+    <v>3.61</v>
+    <v>3.64</v>
+    <v>3.58</v>
+    <v>3.56</v>
+    <v>3.63</v>
+    <v>3.62</v>
+    <v>3.61</v>
+    <v>3.6</v>
+    <v>3.57</v>
+    <v>3.44</v>
+    <v>3.37</v>
+    <v>3.26</v>
+    <v>3.4</v>
+    <v>3.3</v>
+    <v>3.33</v>
+    <v>3.29</v>
+    <v>3.3</v>
+    <v>3.47</v>
+    <v>3.41</v>
+    <v>3.45</v>
+    <v>3.33</v>
+    <v>3.4</v>
+    <v>3.37</v>
+    <v>3.39</v>
+    <v>3.42</v>
+    <v>3.44</v>
+    <v>3.53</v>
+    <v>3.46</v>
+    <v>3.37</v>
+    <v>3.48</v>
+    <v>3.52</v>
+    <v>3.43</v>
+    <v>3.44</v>
+    <v>3.45</v>
+    <v>3.49</v>
+    <v>3.46</v>
+    <v>3.45</v>
+    <v>3.49</v>
+    <v>3.48</v>
+    <v>3.47</v>
+    <v>3.55</v>
+    <v>3.55</v>
+    <v>3.6</v>
+    <v>3.52</v>
+    <v>3.58</v>
+    <v>3.57</v>
+    <v>3.53</v>
+    <v>3.39</v>
+    <v>3.35</v>
+    <v>3.4</v>
+    <v>3.32</v>
+    <v>3.28</v>
+    <v>3.23</v>
+    <v>3.25</v>
+    <v>3.23</v>
+    <v>3.28</v>
+    <v>3.29</v>
+    <v>3.21</v>
+    <v>3.11</v>
+    <v>3</v>
+    <v>2.97</v>
+    <v>3.02</v>
+    <v>2.98</v>
+    <v>2.98</v>
+    <v>3.02</v>
+    <v>3.06</v>
+    <v>3.11</v>
+    <v>3</v>
+    <v>2.96</v>
+    <v>2.91</v>
+    <v>2.93</v>
+    <v>2.84</v>
+    <v>2.86</v>
+    <v>3.28</v>
+    <v>3.15</v>
+    <v>3</v>
+    <v>2.87</v>
+    <v>2.81</v>
+    <v>2.78</v>
+    <v>2.65</v>
+    <v>2.67</v>
+    <v>2.72</v>
+    <v>2.75</v>
+    <v>2.78</v>
+    <v>2.76</v>
+    <v>2.83</v>
+    <v>2.79</v>
+    <v>2.7</v>
+    <v>2.59</v>
+    <v>2.57</v>
+    <v>2.61</v>
+    <v>2.6</v>
+    <v>2.52</v>
+    <v>2.61</v>
+    <v>2.65</v>
+    <v>2.61</v>
+    <v>2.52</v>
+    <v>2.62</v>
+    <v>2.61</v>
+    <v>2.57</v>
+    <v>2.73</v>
+    <v>2.67</v>
+    <v>2.76</v>
+    <v>2.81</v>
+    <v>2.77</v>
+    <v>2.72</v>
+    <v>2.7</v>
+    <v>2.73</v>
+    <v>2.78</v>
+    <v>2.9</v>
+    <v>2.89</v>
+    <v>2.88</v>
+    <v>2.94</v>
+    <v>2.93</v>
+    <v>3</v>
+    <v>2.97</v>
+    <v>2.98</v>
+    <v>2.9</v>
+    <v>2.99</v>
+    <v>2.95</v>
+    <v>2.95</v>
+    <v>2.98</v>
+    <v>3.05</v>
+    <v>3.04</v>
+    <v>3.06</v>
+    <v>2.89</v>
+    <v>2.96</v>
+    <v>3</v>
+    <v>3.01</v>
+    <v>3.03</v>
+    <v>2.96</v>
+    <v>2.95</v>
+    <v>2.95</v>
+    <v>2.85</v>
+    <v>2.82</v>
+    <v>2.83</v>
+    <v>2.84</v>
+    <v>2.76</v>
+    <v>2.77</v>
+    <v>2.78</v>
+    <v>2.81</v>
+    <v>2.85</v>
+    <v>2.77</v>
+    <v>2.74</v>
+    <v>2.75</v>
+    <v>2.75</v>
+    <v>2.77</v>
+    <v>2.71</v>
+    <v>2.62</v>
+    <v>2.6</v>
+    <v>2.56</v>
+    <v>2.6</v>
+    <v>2.66</v>
+    <v>2.67</v>
+    <v>2.66</v>
+    <v>2.76</v>
+    <v>2.94</v>
+    <v>2.9</v>
+    <v>2.86</v>
+    <v>2.79</v>
+    <v>2.79</v>
+    <v>2.75</v>
+    <v>2.66</v>
+    <v>2.72</v>
+    <v>2.56</v>
+    <v>2.5499999999999998</v>
+    <v>2.62</v>
+    <v>2.5299999999999998</v>
+    <v>2.4900000000000002</v>
+    <v>2.5499999999999998</v>
+    <v>2.59</v>
+    <v>2.65</v>
+    <v>2.77</v>
+    <v>2.82</v>
+    <v>2.88</v>
+    <v>2.88</v>
+    <v>2.82</v>
+    <v>2.85</v>
+    <v>2.85</v>
+    <v>2.85</v>
+    <v>2.78</v>
+    <v>2.79</v>
+    <v>2.79</v>
+    <v>2.88</v>
+    <v>2.88</v>
+    <v>2.91</v>
+    <v>2.95</v>
+    <v>2.96</v>
+    <v>2.98</v>
+    <v>3.02</v>
+    <v>2.99</v>
+    <v>3.03</v>
+    <v>3.03</v>
+    <v>3.03</v>
+    <v>3.03</v>
+    <v>3.04</v>
+    <v>3.03</v>
+    <v>3.03</v>
+    <v>3.06</v>
+    <v>3.12</v>
+    <v>3.1</v>
+    <v>3.06</v>
+    <v>3.03</v>
+    <v>3</v>
+    <v>3</v>
+    <v>3.04</v>
+    <v>3.06</v>
+    <v>2.99</v>
+    <v>2.94</v>
+    <v>2.96</v>
+    <v>2.88</v>
+    <v>2.9</v>
+    <v>2.87</v>
+    <v>2.86</v>
+    <v>2.87</v>
+    <v>2.85</v>
+    <v>2.89</v>
+    <v>2.87</v>
+    <v>2.95</v>
+    <v>2.95</v>
+    <v>2.99</v>
+    <v>3.02</v>
+    <v>3.1</v>
+    <v>3.09</v>
+    <v>3.18</v>
+    <v>3.27</v>
+    <v>3.35</v>
+    <v>3.41</v>
+    <v>3.35</v>
+    <v>3.34</v>
+    <v>3.38</v>
+    <v>3.42</v>
+    <v>3.45</v>
+    <v>3.56</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.87</v>
+    <v>2.85</v>
+    <v>2.89</v>
+    <v>2.87</v>
+    <v>2.95</v>
+    <v>2.95</v>
+    <v>2.99</v>
+    <v>3.02</v>
+    <v>3.1</v>
+    <v>3.09</v>
+    <v>3.18</v>
+    <v>3.27</v>
+    <v>3.35</v>
+    <v>3.41</v>
+    <v>3.35</v>
+    <v>3.34</v>
+    <v>3.38</v>
+    <v>3.42</v>
+    <v>3.45</v>
+    <v>3.56</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.87</v>
+    <v>2.84</v>
+    <v>2.86</v>
+    <v>2.91</v>
+    <v>2.9</v>
+    <v>2.93</v>
+    <v>2.95</v>
+    <v>3</v>
+    <v>3.03</v>
+    <v>3.11</v>
+    <v>3.13</v>
+    <v>3.21</v>
+    <v>3.3</v>
+    <v>3.37</v>
+    <v>3.42</v>
+    <v>3.35</v>
+    <v>3.35</v>
+    <v>3.38</v>
+    <v>3.5</v>
+    <v>3.46</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.875</v>
+    <v>2.8849999999999998</v>
+    <v>2.91</v>
+    <v>2.93</v>
+    <v>2.96</v>
+    <v>2.98</v>
+    <v>2.9950000000000001</v>
+    <v>3.0649999999999999</v>
+    <v>3.14</v>
+    <v>3.14</v>
+    <v>3.1850000000000001</v>
+    <v>3.28</v>
+    <v>3.36</v>
+    <v>3.46</v>
+    <v>3.42</v>
+    <v>3.37</v>
+    <v>3.39</v>
+    <v>3.4350000000000001</v>
+    <v>3.58</v>
+    <v>3.57</v>
+  </a>
+  <a r="1" c="20">
+    <v>2.8450000000000002</v>
+    <v>2.84</v>
+    <v>2.86</v>
+    <v>2.8450000000000002</v>
+    <v>2.875</v>
+    <v>2.92</v>
+    <v>2.94</v>
+    <v>2.99</v>
+    <v>3.01</v>
+    <v>3.09</v>
+    <v>3.1</v>
+    <v>3.2</v>
+    <v>3.28</v>
+    <v>3.36</v>
+    <v>3.3149999999999999</v>
+    <v>3.29</v>
+    <v>3.29</v>
+    <v>3.31</v>
+    <v>3.45</v>
+    <v>3.45</v>
+  </a>
+  <a r="1" c="20">
+    <v>302633</v>
+    <v>513658</v>
+    <v>374874</v>
+    <v>471789</v>
+    <v>751911</v>
+    <v>985033</v>
+    <v>453477</v>
+    <v>609942</v>
+    <v>2147656</v>
+    <v>1404152</v>
+    <v>1482589</v>
+    <v>2507185</v>
+    <v>1125033</v>
+    <v>2753760</v>
+    <v>1976616</v>
+    <v>1507511</v>
+    <v>2781223</v>
+    <v>1269223</v>
+    <v>1975775</v>
+    <v>2454922</v>
+  </a>
 </arrayData>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1261">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1374">
   <rv s="0">
     <v>0</v>
     <v>USD/AUD</v>
@@ -25028,6 +26502,450 @@
     <fb>1.75</fb>
     <v>14</v>
   </rv>
+  <rv s="6">
+    <fb>5.68</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>5.95</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>5.87</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>6.21</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>6.45</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>6.53</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.8</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.87</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.95</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.99</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.93</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.79</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.72</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.63</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.71</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.73</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.61</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.64</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.58</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.56</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.62</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.6</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.57</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.44</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.37</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.26</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.4</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.3</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.33</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.29</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.47</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.41</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.45</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.39</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.42</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.53</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.46</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.48</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.52</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.43</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.49</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.55</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.35</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.32</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.23</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.25</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.21</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.11</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.97</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.02</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.06</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.91</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.84</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.15</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.81</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.78</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.67</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.83</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.77</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.9</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.88</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.94</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.99</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.95</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.05</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.04</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.01</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.03</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.82</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.12</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.1</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.09</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.18</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.27</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.34</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.38</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>302633</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.875</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2.8450000000000002</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>513658</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.8849999999999998</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>374874</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>471789</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>751911</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>985033</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.92</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>453477</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2.9950000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>609942</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.0649999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2147656</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1404152</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1482589</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.13</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.1850000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2507185</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.2</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1125033</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.36</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2753760</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1976616</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.3149999999999999</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1507511</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>2781223</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>1269223</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.4350000000000001</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>3.31</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>1975775</fb>
+    <v>15</v>
+  </rv>
+  <rv s="6">
+    <fb>3.5</fb>
+    <v>14</v>
+  </rv>
+  <rv s="6">
+    <fb>2454922</fb>
+    <v>15</v>
+  </rv>
   <rv s="2">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa533m&amp;q=XASX%3aBLD&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -25060,7 +26978,7 @@
     <v>Construction Materials</v>
     <v>Stock</v>
     <v>44951.333344907405</v>
-    <v>1248</v>
+    <v>1359</v>
     <v>3.45</v>
     <v>3805655000</v>
     <v>BORAL LIMITED</v>
@@ -25077,7 +26995,7 @@
     <v>1960</v>
   </rv>
   <rv s="1">
-    <v>1249</v>
+    <v>1360</v>
   </rv>
   <rv s="2">
     <v>https://www.bing.com/financeapi/forcetrigger?t=aa4om7&amp;q=XASX%3aASB&amp;form=skydnc</v>
@@ -25111,7 +27029,7 @@
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
     <v>44951.333333333336</v>
-    <v>1251</v>
+    <v>1362</v>
     <v>1.6950000000000001</v>
     <v>639709900</v>
     <v>AUSTAL LIMITED</v>
@@ -25128,7 +27046,7 @@
     <v>1987</v>
   </rv>
   <rv s="1">
-    <v>1252</v>
+    <v>1363</v>
   </rv>
   <rv s="8">
     <v>16</v>
@@ -25231,6 +27149,38 @@
     <v>aa658m</v>
     <v>XASX:EOS</v>
     <v>12</v>
+  </rv>
+  <rv s="8">
+    <v>16</v>
+    <v>XASX:BLD</v>
+    <v>Daily</v>
+    <v>44587</v>
+    <v>44952</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638102016000000000,638102735671464712,0</v>
+    <v>0</v>
+    <v>aa533m</v>
+    <v>XASX:BLD</v>
+    <v>13</v>
+  </rv>
+  <rv s="9">
+    <v>17</v>
+    <v>XASX:BLD</v>
+    <v>Daily</v>
+    <v>44922</v>
+    <v>44952</v>
+    <v>0</v>
+    <v>1</v>
+    <v>638102016000000000,638102735834809227,0</v>
+    <v>2</v>
+    <v>aa533m</v>
+    <v>XASX:BLD</v>
+    <v>14</v>
+    <v>15</v>
+    <v>16</v>
+    <v>17</v>
+    <v>18</v>
   </rv>
 </rvData>
 </file>
@@ -26306,7 +28256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -33530,8 +35480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65173A22-D60C-684F-AC10-940F91797BDE}">
   <dimension ref="A1:IT26"/>
   <sheetViews>
-    <sheetView topLeftCell="DX1" workbookViewId="0">
-      <selection activeCell="HF23" sqref="HF23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35124,16 +37074,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38F13E4-FF82-6E40-B343-A0462498EE32}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:IT27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -35141,7 +37093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -35149,12 +37101,1566 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:254" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
+      </c>
+      <c r="C4" cm="1" vm="1232">
+        <f t="array" aca="1" ref="C4:IT4" ca="1">TRANSPOSE(_xlfn.STOCKHISTORY(A4&amp;":"&amp;B4, TODAY()-365, TODAY(),0,0,1))</f>
+        <v>5.68</v>
+      </c>
+      <c r="D4" vm="1233">
+        <f ca="1"/>
+        <v>5.95</v>
+      </c>
+      <c r="E4" vm="1234">
+        <f ca="1"/>
+        <v>5.87</v>
+      </c>
+      <c r="F4" vm="1235">
+        <f ca="1"/>
+        <v>6.21</v>
+      </c>
+      <c r="G4" vm="1236">
+        <f ca="1"/>
+        <v>6.45</v>
+      </c>
+      <c r="H4" vm="1237">
+        <f ca="1"/>
+        <v>6.53</v>
+      </c>
+      <c r="I4" vm="1238">
+        <f ca="1"/>
+        <v>3.8</v>
+      </c>
+      <c r="J4" vm="1239">
+        <f ca="1"/>
+        <v>3.87</v>
+      </c>
+      <c r="K4" vm="1240">
+        <f ca="1"/>
+        <v>3.95</v>
+      </c>
+      <c r="L4" vm="1241">
+        <f ca="1"/>
+        <v>3.99</v>
+      </c>
+      <c r="M4" vm="1242">
+        <f ca="1"/>
+        <v>3.93</v>
+      </c>
+      <c r="N4" vm="1243">
+        <f ca="1"/>
+        <v>3.79</v>
+      </c>
+      <c r="O4" vm="1244">
+        <f ca="1"/>
+        <v>3.72</v>
+      </c>
+      <c r="P4" vm="1245">
+        <f ca="1"/>
+        <v>3.63</v>
+      </c>
+      <c r="Q4" vm="1246">
+        <f ca="1"/>
+        <v>3.71</v>
+      </c>
+      <c r="R4" vm="1247">
+        <f ca="1"/>
+        <v>3.73</v>
+      </c>
+      <c r="S4" vm="1246">
+        <f ca="1"/>
+        <v>3.71</v>
+      </c>
+      <c r="T4" vm="1246">
+        <f ca="1"/>
+        <v>3.71</v>
+      </c>
+      <c r="U4" vm="1248">
+        <f ca="1"/>
+        <v>3.61</v>
+      </c>
+      <c r="V4" vm="1249">
+        <f ca="1"/>
+        <v>3.64</v>
+      </c>
+      <c r="W4" vm="1250">
+        <f ca="1"/>
+        <v>3.58</v>
+      </c>
+      <c r="X4" vm="1251">
+        <f ca="1"/>
+        <v>3.56</v>
+      </c>
+      <c r="Y4" vm="1245">
+        <f ca="1"/>
+        <v>3.63</v>
+      </c>
+      <c r="Z4" vm="1252">
+        <f ca="1"/>
+        <v>3.62</v>
+      </c>
+      <c r="AA4" vm="1248">
+        <f ca="1"/>
+        <v>3.61</v>
+      </c>
+      <c r="AB4" vm="1253">
+        <f ca="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="AC4" vm="1254">
+        <f ca="1"/>
+        <v>3.57</v>
+      </c>
+      <c r="AD4" vm="1255">
+        <f ca="1"/>
+        <v>3.44</v>
+      </c>
+      <c r="AE4" vm="1256">
+        <f ca="1"/>
+        <v>3.37</v>
+      </c>
+      <c r="AF4" vm="1257">
+        <f ca="1"/>
+        <v>3.26</v>
+      </c>
+      <c r="AG4" vm="1258">
+        <f ca="1"/>
+        <v>3.4</v>
+      </c>
+      <c r="AH4" vm="1259">
+        <f ca="1"/>
+        <v>3.3</v>
+      </c>
+      <c r="AI4" vm="1260">
+        <f ca="1"/>
+        <v>3.33</v>
+      </c>
+      <c r="AJ4" vm="1261">
+        <f ca="1"/>
+        <v>3.29</v>
+      </c>
+      <c r="AK4" vm="1259">
+        <f ca="1"/>
+        <v>3.3</v>
+      </c>
+      <c r="AL4" vm="1262">
+        <f ca="1"/>
+        <v>3.47</v>
+      </c>
+      <c r="AM4" vm="1263">
+        <f ca="1"/>
+        <v>3.41</v>
+      </c>
+      <c r="AN4" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="AO4" vm="1260">
+        <f ca="1"/>
+        <v>3.33</v>
+      </c>
+      <c r="AP4" vm="1258">
+        <f ca="1"/>
+        <v>3.4</v>
+      </c>
+      <c r="AQ4" vm="1256">
+        <f ca="1"/>
+        <v>3.37</v>
+      </c>
+      <c r="AR4" vm="1265">
+        <f ca="1"/>
+        <v>3.39</v>
+      </c>
+      <c r="AS4" vm="1266">
+        <f ca="1"/>
+        <v>3.42</v>
+      </c>
+      <c r="AT4" vm="1255">
+        <f ca="1"/>
+        <v>3.44</v>
+      </c>
+      <c r="AU4" vm="1267">
+        <f ca="1"/>
+        <v>3.53</v>
+      </c>
+      <c r="AV4" vm="1268">
+        <f ca="1"/>
+        <v>3.46</v>
+      </c>
+      <c r="AW4" vm="1256">
+        <f ca="1"/>
+        <v>3.37</v>
+      </c>
+      <c r="AX4" vm="1269">
+        <f ca="1"/>
+        <v>3.48</v>
+      </c>
+      <c r="AY4" vm="1270">
+        <f ca="1"/>
+        <v>3.52</v>
+      </c>
+      <c r="AZ4" vm="1271">
+        <f ca="1"/>
+        <v>3.43</v>
+      </c>
+      <c r="BA4" vm="1255">
+        <f ca="1"/>
+        <v>3.44</v>
+      </c>
+      <c r="BB4" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="BC4" vm="1272">
+        <f ca="1"/>
+        <v>3.49</v>
+      </c>
+      <c r="BD4" vm="1268">
+        <f ca="1"/>
+        <v>3.46</v>
+      </c>
+      <c r="BE4" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="BF4" vm="1272">
+        <f ca="1"/>
+        <v>3.49</v>
+      </c>
+      <c r="BG4" vm="1269">
+        <f ca="1"/>
+        <v>3.48</v>
+      </c>
+      <c r="BH4" vm="1262">
+        <f ca="1"/>
+        <v>3.47</v>
+      </c>
+      <c r="BI4" vm="1273">
+        <f ca="1"/>
+        <v>3.55</v>
+      </c>
+      <c r="BJ4" vm="1273">
+        <f ca="1"/>
+        <v>3.55</v>
+      </c>
+      <c r="BK4" vm="1253">
+        <f ca="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="BL4" vm="1270">
+        <f ca="1"/>
+        <v>3.52</v>
+      </c>
+      <c r="BM4" vm="1250">
+        <f ca="1"/>
+        <v>3.58</v>
+      </c>
+      <c r="BN4" vm="1254">
+        <f ca="1"/>
+        <v>3.57</v>
+      </c>
+      <c r="BO4" vm="1267">
+        <f ca="1"/>
+        <v>3.53</v>
+      </c>
+      <c r="BP4" vm="1265">
+        <f ca="1"/>
+        <v>3.39</v>
+      </c>
+      <c r="BQ4" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+      <c r="BR4" vm="1258">
+        <f ca="1"/>
+        <v>3.4</v>
+      </c>
+      <c r="BS4" vm="1275">
+        <f ca="1"/>
+        <v>3.32</v>
+      </c>
+      <c r="BT4" vm="867">
+        <f ca="1"/>
+        <v>3.28</v>
+      </c>
+      <c r="BU4" vm="1276">
+        <f ca="1"/>
+        <v>3.23</v>
+      </c>
+      <c r="BV4" vm="1277">
+        <f ca="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="BW4" vm="1276">
+        <f ca="1"/>
+        <v>3.23</v>
+      </c>
+      <c r="BX4" vm="867">
+        <f ca="1"/>
+        <v>3.28</v>
+      </c>
+      <c r="BY4" vm="1261">
+        <f ca="1"/>
+        <v>3.29</v>
+      </c>
+      <c r="BZ4" vm="1278">
+        <f ca="1"/>
+        <v>3.21</v>
+      </c>
+      <c r="CA4" vm="1279">
+        <f ca="1"/>
+        <v>3.11</v>
+      </c>
+      <c r="CB4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="CC4" vm="1281">
+        <f ca="1"/>
+        <v>2.97</v>
+      </c>
+      <c r="CD4" vm="1282">
+        <f ca="1"/>
+        <v>3.02</v>
+      </c>
+      <c r="CE4" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="CF4" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="CG4" vm="1282">
+        <f ca="1"/>
+        <v>3.02</v>
+      </c>
+      <c r="CH4" vm="1283">
+        <f ca="1"/>
+        <v>3.06</v>
+      </c>
+      <c r="CI4" vm="1279">
+        <f ca="1"/>
+        <v>3.11</v>
+      </c>
+      <c r="CJ4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="CK4" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="CL4" vm="1284">
+        <f ca="1"/>
+        <v>2.91</v>
+      </c>
+      <c r="CM4" vm="869">
+        <f ca="1"/>
+        <v>2.93</v>
+      </c>
+      <c r="CN4" vm="1285">
+        <f ca="1"/>
+        <v>2.84</v>
+      </c>
+      <c r="CO4" vm="871">
+        <f ca="1"/>
+        <v>2.86</v>
+      </c>
+      <c r="CP4" vm="867">
+        <f ca="1"/>
+        <v>3.28</v>
+      </c>
+      <c r="CQ4" vm="1286">
+        <f ca="1"/>
+        <v>3.15</v>
+      </c>
+      <c r="CR4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="CS4" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+      <c r="CT4" vm="1287">
+        <f ca="1"/>
+        <v>2.81</v>
+      </c>
+      <c r="CU4" vm="1288">
+        <f ca="1"/>
+        <v>2.78</v>
+      </c>
+      <c r="CV4" vm="878">
+        <f ca="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="CW4" vm="1289">
+        <f ca="1"/>
+        <v>2.67</v>
+      </c>
+      <c r="CX4" vm="864">
+        <f ca="1"/>
+        <v>2.72</v>
+      </c>
+      <c r="CY4" vm="870">
+        <f ca="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="CZ4" vm="1288">
+        <f ca="1"/>
+        <v>2.78</v>
+      </c>
+      <c r="DA4" vm="1179">
+        <f ca="1"/>
+        <v>2.76</v>
+      </c>
+      <c r="DB4" vm="1290">
+        <f ca="1"/>
+        <v>2.83</v>
+      </c>
+      <c r="DC4" vm="877">
+        <f ca="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="DD4" vm="874">
+        <f ca="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="DE4" vm="1182">
+        <f ca="1"/>
+        <v>2.59</v>
+      </c>
+      <c r="DF4" vm="1171">
+        <f ca="1"/>
+        <v>2.57</v>
+      </c>
+      <c r="DG4" vm="1181">
+        <f ca="1"/>
+        <v>2.61</v>
+      </c>
+      <c r="DH4" vm="1180">
+        <f ca="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="DI4" vm="1183">
+        <f ca="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="DJ4" vm="1181">
+        <f ca="1"/>
+        <v>2.61</v>
+      </c>
+      <c r="DK4" vm="878">
+        <f ca="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="DL4" vm="1181">
+        <f ca="1"/>
+        <v>2.61</v>
+      </c>
+      <c r="DM4" vm="1183">
+        <f ca="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="DN4" vm="1172">
+        <f ca="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="DO4" vm="1181">
+        <f ca="1"/>
+        <v>2.61</v>
+      </c>
+      <c r="DP4" vm="1171">
+        <f ca="1"/>
+        <v>2.57</v>
+      </c>
+      <c r="DQ4" vm="1176">
+        <f ca="1"/>
+        <v>2.73</v>
+      </c>
+      <c r="DR4" vm="1289">
+        <f ca="1"/>
+        <v>2.67</v>
+      </c>
+      <c r="DS4" vm="1179">
+        <f ca="1"/>
+        <v>2.76</v>
+      </c>
+      <c r="DT4" vm="1287">
+        <f ca="1"/>
+        <v>2.81</v>
+      </c>
+      <c r="DU4" vm="1291">
+        <f ca="1"/>
+        <v>2.77</v>
+      </c>
+      <c r="DV4" vm="864">
+        <f ca="1"/>
+        <v>2.72</v>
+      </c>
+      <c r="DW4" vm="874">
+        <f ca="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="DX4" vm="1176">
+        <f ca="1"/>
+        <v>2.73</v>
+      </c>
+      <c r="DY4" vm="1288">
+        <f ca="1"/>
+        <v>2.78</v>
+      </c>
+      <c r="DZ4" vm="1292">
+        <f ca="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="EA4" vm="868">
+        <f ca="1"/>
+        <v>2.89</v>
+      </c>
+      <c r="EB4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="EC4" vm="1294">
+        <f ca="1"/>
+        <v>2.94</v>
+      </c>
+      <c r="ED4" vm="869">
+        <f ca="1"/>
+        <v>2.93</v>
+      </c>
+      <c r="EE4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="EF4" vm="1281">
+        <f ca="1"/>
+        <v>2.97</v>
+      </c>
+      <c r="EG4" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="EH4" vm="1292">
+        <f ca="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="EI4" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+      <c r="EJ4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="EK4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="EL4" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="EM4" vm="1297">
+        <f ca="1"/>
+        <v>3.05</v>
+      </c>
+      <c r="EN4" vm="1298">
+        <f ca="1"/>
+        <v>3.04</v>
+      </c>
+      <c r="EO4" vm="1283">
+        <f ca="1"/>
+        <v>3.06</v>
+      </c>
+      <c r="EP4" vm="868">
+        <f ca="1"/>
+        <v>2.89</v>
+      </c>
+      <c r="EQ4" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="ER4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="ES4" vm="1299">
+        <f ca="1"/>
+        <v>3.01</v>
+      </c>
+      <c r="ET4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="EU4" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="EV4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="EW4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="EX4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="EY4" vm="1301">
+        <f ca="1"/>
+        <v>2.82</v>
+      </c>
+      <c r="EZ4" vm="1290">
+        <f ca="1"/>
+        <v>2.83</v>
+      </c>
+      <c r="FA4" vm="1285">
+        <f ca="1"/>
+        <v>2.84</v>
+      </c>
+      <c r="FB4" vm="1179">
+        <f ca="1"/>
+        <v>2.76</v>
+      </c>
+      <c r="FC4" vm="1291">
+        <f ca="1"/>
+        <v>2.77</v>
+      </c>
+      <c r="FD4" vm="1288">
+        <f ca="1"/>
+        <v>2.78</v>
+      </c>
+      <c r="FE4" vm="1287">
+        <f ca="1"/>
+        <v>2.81</v>
+      </c>
+      <c r="FF4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="FG4" vm="1291">
+        <f ca="1"/>
+        <v>2.77</v>
+      </c>
+      <c r="FH4" vm="875">
+        <f ca="1"/>
+        <v>2.74</v>
+      </c>
+      <c r="FI4" vm="870">
+        <f ca="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="FJ4" vm="870">
+        <f ca="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="FK4" vm="1291">
+        <f ca="1"/>
+        <v>2.77</v>
+      </c>
+      <c r="FL4" vm="1178">
+        <f ca="1"/>
+        <v>2.71</v>
+      </c>
+      <c r="FM4" vm="1172">
+        <f ca="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="FN4" vm="1180">
+        <f ca="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="FO4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="FP4" vm="1180">
+        <f ca="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="FQ4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="FR4" vm="1289">
+        <f ca="1"/>
+        <v>2.67</v>
+      </c>
+      <c r="FS4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="FT4" vm="1179">
+        <f ca="1"/>
+        <v>2.76</v>
+      </c>
+      <c r="FU4" vm="1294">
+        <f ca="1"/>
+        <v>2.94</v>
+      </c>
+      <c r="FV4" vm="1292">
+        <f ca="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="FW4" vm="871">
+        <f ca="1"/>
+        <v>2.86</v>
+      </c>
+      <c r="FX4" vm="877">
+        <f ca="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="FY4" vm="877">
+        <f ca="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="FZ4" vm="870">
+        <f ca="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="GA4" vm="1175">
+        <f ca="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="GB4" vm="864">
+        <f ca="1"/>
+        <v>2.72</v>
+      </c>
+      <c r="GC4" vm="1166">
+        <f ca="1"/>
+        <v>2.56</v>
+      </c>
+      <c r="GD4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="GE4" vm="1172">
+        <f ca="1"/>
+        <v>2.62</v>
+      </c>
+      <c r="GF4" vm="1170">
+        <f ca="1"/>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="GG4" vm="1169">
+        <f ca="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="GH4" vm="1167">
+        <f ca="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="GI4" vm="1182">
+        <f ca="1"/>
+        <v>2.59</v>
+      </c>
+      <c r="GJ4" vm="878">
+        <f ca="1"/>
+        <v>2.65</v>
+      </c>
+      <c r="GK4" vm="1291">
+        <f ca="1"/>
+        <v>2.77</v>
+      </c>
+      <c r="GL4" vm="1301">
+        <f ca="1"/>
+        <v>2.82</v>
+      </c>
+      <c r="GM4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="GN4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="GO4" vm="1301">
+        <f ca="1"/>
+        <v>2.82</v>
+      </c>
+      <c r="GP4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="GQ4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="GR4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="GS4" vm="1288">
+        <f ca="1"/>
+        <v>2.78</v>
+      </c>
+      <c r="GT4" vm="877">
+        <f ca="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="GU4" vm="877">
+        <f ca="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="GV4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="GW4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="GX4" vm="1284">
+        <f ca="1"/>
+        <v>2.91</v>
+      </c>
+      <c r="GY4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="GZ4" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="HA4" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="HB4" vm="1282">
+        <f ca="1"/>
+        <v>3.02</v>
+      </c>
+      <c r="HC4" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+      <c r="HD4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HE4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HF4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HG4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HH4" vm="1298">
+        <f ca="1"/>
+        <v>3.04</v>
+      </c>
+      <c r="HI4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HJ4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HK4" vm="1283">
+        <f ca="1"/>
+        <v>3.06</v>
+      </c>
+      <c r="HL4" vm="1302">
+        <f ca="1"/>
+        <v>3.12</v>
+      </c>
+      <c r="HM4" vm="1303">
+        <f ca="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="HN4" vm="1283">
+        <f ca="1"/>
+        <v>3.06</v>
+      </c>
+      <c r="HO4" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="HP4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="HQ4" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="HR4" vm="1298">
+        <f ca="1"/>
+        <v>3.04</v>
+      </c>
+      <c r="HS4" vm="1283">
+        <f ca="1"/>
+        <v>3.06</v>
+      </c>
+      <c r="HT4" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+      <c r="HU4" vm="1294">
+        <f ca="1"/>
+        <v>2.94</v>
+      </c>
+      <c r="HV4" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="HW4" vm="1293">
+        <f ca="1"/>
+        <v>2.88</v>
+      </c>
+      <c r="HX4" vm="1292">
+        <f ca="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="HY4" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+      <c r="HZ4" vm="871">
+        <f ca="1"/>
+        <v>2.86</v>
+      </c>
+      <c r="IA4" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+      <c r="IB4" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="IC4" vm="868">
+        <f ca="1"/>
+        <v>2.89</v>
+      </c>
+      <c r="ID4" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+      <c r="IE4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="IF4" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="IG4" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+      <c r="IH4" vm="1282">
+        <f ca="1"/>
+        <v>3.02</v>
+      </c>
+      <c r="II4" vm="1303">
+        <f ca="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="IJ4" vm="1304">
+        <f ca="1"/>
+        <v>3.09</v>
+      </c>
+      <c r="IK4" vm="1305">
+        <f ca="1"/>
+        <v>3.18</v>
+      </c>
+      <c r="IL4" vm="1306">
+        <f ca="1"/>
+        <v>3.27</v>
+      </c>
+      <c r="IM4" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+      <c r="IN4" vm="1263">
+        <f ca="1"/>
+        <v>3.41</v>
+      </c>
+      <c r="IO4" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+      <c r="IP4" vm="1307">
+        <f ca="1"/>
+        <v>3.34</v>
+      </c>
+      <c r="IQ4" vm="1308">
+        <f ca="1"/>
+        <v>3.38</v>
+      </c>
+      <c r="IR4" vm="1266">
+        <f ca="1"/>
+        <v>3.42</v>
+      </c>
+      <c r="IS4" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="IT4" vm="1251">
+        <f ca="1"/>
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A7" t="str" cm="1">
+        <f t="array" aca="1" ref="A7:F27" ca="1">(_xlfn.STOCKHISTORY(A4&amp;":"&amp;B4, TODAY()-30, TODAY(),0,1,0,5,2,3,4,1))</f>
+        <v>Date</v>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1"/>
+        <v>Volume</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1"/>
+        <v>Open</v>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1"/>
+        <v>High</v>
+      </c>
+      <c r="E7" t="str">
+        <f ca="1"/>
+        <v>Low</v>
+      </c>
+      <c r="F7" t="str">
+        <f ca="1"/>
+        <v>Close</v>
+      </c>
+    </row>
+    <row r="8" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A8" vm="242">
+        <f ca="1"/>
+        <v>44923</v>
+      </c>
+      <c r="B8" vm="1309">
+        <f ca="1"/>
+        <v>302633</v>
+      </c>
+      <c r="C8" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+      <c r="D8" vm="1310">
+        <f ca="1"/>
+        <v>2.875</v>
+      </c>
+      <c r="E8" vm="1311">
+        <f ca="1"/>
+        <v>2.8450000000000002</v>
+      </c>
+      <c r="F8" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A9" vm="243">
+        <f ca="1"/>
+        <v>44924</v>
+      </c>
+      <c r="B9" vm="1312">
+        <f ca="1"/>
+        <v>513658</v>
+      </c>
+      <c r="C9" vm="1285">
+        <f ca="1"/>
+        <v>2.84</v>
+      </c>
+      <c r="D9" vm="1313">
+        <f ca="1"/>
+        <v>2.8849999999999998</v>
+      </c>
+      <c r="E9" vm="1285">
+        <f ca="1"/>
+        <v>2.84</v>
+      </c>
+      <c r="F9" vm="876">
+        <f ca="1"/>
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A10" vm="244">
+        <f ca="1"/>
+        <v>44925</v>
+      </c>
+      <c r="B10" vm="1314">
+        <f ca="1"/>
+        <v>374874</v>
+      </c>
+      <c r="C10" vm="871">
+        <f ca="1"/>
+        <v>2.86</v>
+      </c>
+      <c r="D10" vm="1284">
+        <f ca="1"/>
+        <v>2.91</v>
+      </c>
+      <c r="E10" vm="871">
+        <f ca="1"/>
+        <v>2.86</v>
+      </c>
+      <c r="F10" vm="868">
+        <f ca="1"/>
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A11" vm="245">
+        <f ca="1"/>
+        <v>44929</v>
+      </c>
+      <c r="B11" vm="1315">
+        <f ca="1"/>
+        <v>471789</v>
+      </c>
+      <c r="C11" vm="1284">
+        <f ca="1"/>
+        <v>2.91</v>
+      </c>
+      <c r="D11" vm="869">
+        <f ca="1"/>
+        <v>2.93</v>
+      </c>
+      <c r="E11" vm="1311">
+        <f ca="1"/>
+        <v>2.8450000000000002</v>
+      </c>
+      <c r="F11" vm="873">
+        <f ca="1"/>
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A12" vm="246">
+        <f ca="1"/>
+        <v>44930</v>
+      </c>
+      <c r="B12" vm="1316">
+        <f ca="1"/>
+        <v>751911</v>
+      </c>
+      <c r="C12" vm="1292">
+        <f ca="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="D12" vm="872">
+        <f ca="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="E12" vm="1310">
+        <f ca="1"/>
+        <v>2.875</v>
+      </c>
+      <c r="F12" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A13" vm="247">
+        <f ca="1"/>
+        <v>44931</v>
+      </c>
+      <c r="B13" vm="1317">
+        <f ca="1"/>
+        <v>985033</v>
+      </c>
+      <c r="C13" vm="869">
+        <f ca="1"/>
+        <v>2.93</v>
+      </c>
+      <c r="D13" vm="865">
+        <f ca="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="E13" vm="1318">
+        <f ca="1"/>
+        <v>2.92</v>
+      </c>
+      <c r="F13" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A14" vm="248">
+        <f ca="1"/>
+        <v>44932</v>
+      </c>
+      <c r="B14" vm="1319">
+        <f ca="1"/>
+        <v>453477</v>
+      </c>
+      <c r="C14" vm="1296">
+        <f ca="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="D14" vm="1320">
+        <f ca="1"/>
+        <v>2.9950000000000001</v>
+      </c>
+      <c r="E14" vm="1294">
+        <f ca="1"/>
+        <v>2.94</v>
+      </c>
+      <c r="F14" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A15" vm="249">
+        <f ca="1"/>
+        <v>44935</v>
+      </c>
+      <c r="B15" vm="1321">
+        <f ca="1"/>
+        <v>609942</v>
+      </c>
+      <c r="C15" vm="1280">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="D15" vm="1322">
+        <f ca="1"/>
+        <v>3.0649999999999999</v>
+      </c>
+      <c r="E15" vm="1295">
+        <f ca="1"/>
+        <v>2.99</v>
+      </c>
+      <c r="F15" vm="1282">
+        <f ca="1"/>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:254" x14ac:dyDescent="0.2">
+      <c r="A16" vm="250">
+        <f ca="1"/>
+        <v>44936</v>
+      </c>
+      <c r="B16" vm="1323">
+        <f ca="1"/>
+        <v>2147656</v>
+      </c>
+      <c r="C16" vm="1300">
+        <f ca="1"/>
+        <v>3.03</v>
+      </c>
+      <c r="D16" vm="866">
+        <f ca="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="E16" vm="1299">
+        <f ca="1"/>
+        <v>3.01</v>
+      </c>
+      <c r="F16" vm="1303">
+        <f ca="1"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" vm="251">
+        <f ca="1"/>
+        <v>44937</v>
+      </c>
+      <c r="B17" vm="1324">
+        <f ca="1"/>
+        <v>1404152</v>
+      </c>
+      <c r="C17" vm="1279">
+        <f ca="1"/>
+        <v>3.11</v>
+      </c>
+      <c r="D17" vm="866">
+        <f ca="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="E17" vm="1304">
+        <f ca="1"/>
+        <v>3.09</v>
+      </c>
+      <c r="F17" vm="1304">
+        <f ca="1"/>
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" vm="252">
+        <f ca="1"/>
+        <v>44938</v>
+      </c>
+      <c r="B18" vm="1325">
+        <f ca="1"/>
+        <v>1482589</v>
+      </c>
+      <c r="C18" vm="1326">
+        <f ca="1"/>
+        <v>3.13</v>
+      </c>
+      <c r="D18" vm="1327">
+        <f ca="1"/>
+        <v>3.1850000000000001</v>
+      </c>
+      <c r="E18" vm="1303">
+        <f ca="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="F18" vm="1305">
+        <f ca="1"/>
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" vm="253">
+        <f ca="1"/>
+        <v>44939</v>
+      </c>
+      <c r="B19" vm="1328">
+        <f ca="1"/>
+        <v>2507185</v>
+      </c>
+      <c r="C19" vm="1278">
+        <f ca="1"/>
+        <v>3.21</v>
+      </c>
+      <c r="D19" vm="867">
+        <f ca="1"/>
+        <v>3.28</v>
+      </c>
+      <c r="E19" vm="1329">
+        <f ca="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="F19" vm="1306">
+        <f ca="1"/>
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" vm="254">
+        <f ca="1"/>
+        <v>44942</v>
+      </c>
+      <c r="B20" vm="1330">
+        <f ca="1"/>
+        <v>1125033</v>
+      </c>
+      <c r="C20" vm="1259">
+        <f ca="1"/>
+        <v>3.3</v>
+      </c>
+      <c r="D20" vm="1331">
+        <f ca="1"/>
+        <v>3.36</v>
+      </c>
+      <c r="E20" vm="867">
+        <f ca="1"/>
+        <v>3.28</v>
+      </c>
+      <c r="F20" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" vm="255">
+        <f ca="1"/>
+        <v>44943</v>
+      </c>
+      <c r="B21" vm="1332">
+        <f ca="1"/>
+        <v>2753760</v>
+      </c>
+      <c r="C21" vm="1256">
+        <f ca="1"/>
+        <v>3.37</v>
+      </c>
+      <c r="D21" vm="1268">
+        <f ca="1"/>
+        <v>3.46</v>
+      </c>
+      <c r="E21" vm="1331">
+        <f ca="1"/>
+        <v>3.36</v>
+      </c>
+      <c r="F21" vm="1263">
+        <f ca="1"/>
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" vm="256">
+        <f ca="1"/>
+        <v>44944</v>
+      </c>
+      <c r="B22" vm="1333">
+        <f ca="1"/>
+        <v>1976616</v>
+      </c>
+      <c r="C22" vm="1266">
+        <f ca="1"/>
+        <v>3.42</v>
+      </c>
+      <c r="D22" vm="1266">
+        <f ca="1"/>
+        <v>3.42</v>
+      </c>
+      <c r="E22" vm="1334">
+        <f ca="1"/>
+        <v>3.3149999999999999</v>
+      </c>
+      <c r="F22" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" vm="257">
+        <f ca="1"/>
+        <v>44945</v>
+      </c>
+      <c r="B23" vm="1335">
+        <f ca="1"/>
+        <v>1507511</v>
+      </c>
+      <c r="C23" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+      <c r="D23" vm="1256">
+        <f ca="1"/>
+        <v>3.37</v>
+      </c>
+      <c r="E23" vm="1261">
+        <f ca="1"/>
+        <v>3.29</v>
+      </c>
+      <c r="F23" vm="1307">
+        <f ca="1"/>
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" vm="258">
+        <f ca="1"/>
+        <v>44946</v>
+      </c>
+      <c r="B24" vm="1336">
+        <f ca="1"/>
+        <v>2781223</v>
+      </c>
+      <c r="C24" vm="1274">
+        <f ca="1"/>
+        <v>3.35</v>
+      </c>
+      <c r="D24" vm="1265">
+        <f ca="1"/>
+        <v>3.39</v>
+      </c>
+      <c r="E24" vm="1261">
+        <f ca="1"/>
+        <v>3.29</v>
+      </c>
+      <c r="F24" vm="1308">
+        <f ca="1"/>
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" vm="259">
+        <f ca="1"/>
+        <v>44949</v>
+      </c>
+      <c r="B25" vm="1337">
+        <f ca="1"/>
+        <v>1269223</v>
+      </c>
+      <c r="C25" vm="1308">
+        <f ca="1"/>
+        <v>3.38</v>
+      </c>
+      <c r="D25" vm="1338">
+        <f ca="1"/>
+        <v>3.4350000000000001</v>
+      </c>
+      <c r="E25" vm="1339">
+        <f ca="1"/>
+        <v>3.31</v>
+      </c>
+      <c r="F25" vm="1266">
+        <f ca="1"/>
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" vm="260">
+        <f ca="1"/>
+        <v>44950</v>
+      </c>
+      <c r="B26" vm="1340">
+        <f ca="1"/>
+        <v>1975775</v>
+      </c>
+      <c r="C26" vm="1341">
+        <f ca="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="D26" vm="1250">
+        <f ca="1"/>
+        <v>3.58</v>
+      </c>
+      <c r="E26" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="F26" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" vm="261">
+        <f ca="1"/>
+        <v>44951</v>
+      </c>
+      <c r="B27" vm="1342">
+        <f ca="1"/>
+        <v>2454922</v>
+      </c>
+      <c r="C27" vm="1268">
+        <f ca="1"/>
+        <v>3.46</v>
+      </c>
+      <c r="D27" vm="1254">
+        <f ca="1"/>
+        <v>3.57</v>
+      </c>
+      <c r="E27" vm="1264">
+        <f ca="1"/>
+        <v>3.45</v>
+      </c>
+      <c r="F27" vm="1251">
+        <f ca="1"/>
+        <v>3.56</v>
       </c>
     </row>
   </sheetData>
@@ -35206,7 +38712,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="e" vm="1232">
+      <c r="A3" t="e" vm="1343">
         <v>#VALUE!</v>
       </c>
       <c r="B3" t="str" cm="1">
@@ -35239,7 +38745,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="e" vm="1233">
+      <c r="A4" t="e" vm="1344">
         <v>#VALUE!</v>
       </c>
       <c r="B4" t="str" cm="1">

</xml_diff>

<commit_message>
Added stock chart for BLD
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EB2681-BB1B-D84A-AF4C-B3B27D36CAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948D0F8F-7549-3040-9E41-2999B0AFDC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="4" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="16" r:id="rId1"/>
@@ -16622,6 +16622,1252 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>BLD!$B$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>BORAL LIMITED (XASX:BLD)</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BLD!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Volume</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>BLD!$A$8:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$B$8:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>302633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>513658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>374874</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>471789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>751911</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>985033</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>453477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>609942</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2147656</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1404152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1482589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2507185</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1125033</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2753760</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1976616</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1507511</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2781223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1269223</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1975775</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2454922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FB0-4E42-B757-8BF0C4176C1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1519738256"/>
+        <c:axId val="1509068912"/>
+      </c:barChart>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BLD!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Open</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BLD!$A$8:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$C$8:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5FB0-4E42-B757-8BF0C4176C1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BLD!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BLD!$A$8:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$D$8:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5FB0-4E42-B757-8BF0C4176C1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BLD!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BLD!$A$8:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$E$8:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.8450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5FB0-4E42-B757-8BF0C4176C1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BLD!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Close</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BLD!$A$8:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$F$8:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5FB0-4E42-B757-8BF0C4176C1F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
+        <c:axId val="1524419888"/>
+        <c:axId val="1524430208"/>
+      </c:stockChart>
+      <c:dateAx>
+        <c:axId val="1519738256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1509068912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1509068912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0,,&quot;M&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519738256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1524430208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524419888"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dateAx>
+        <c:axId val="1524419888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1524430208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -16700,6 +17946,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -18295,6 +19581,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -18404,6 +20206,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>35278</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>35276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F741FA8-6AD3-7F4C-87CB-FF3E4E185F01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -21188,18 +23028,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.6205000000000001</v>
     <v>1.3048</v>
-    <v>-1.11E-2</v>
-    <v>-7.8239999999999994E-3</v>
+    <v>-1.1299999999999999E-2</v>
+    <v>-7.9640000000000006E-3</v>
     <v>AUD</v>
     <v>USD</v>
     <v>1.4218999999999999</v>
     <v>Currency Pair</v>
-    <v>44951.831678240742</v>
+    <v>44951.835393518515</v>
     <v>1.4040999999999999</v>
     <v>US Dollar/Australian Dollar FX Cross Rate</v>
     <v>1.4186000000000001</v>
     <v>1.4188000000000001</v>
-    <v>1.4077</v>
+    <v>1.4075</v>
     <v>USDAUD</v>
     <v>USD/AUD</v>
   </rv>
@@ -28256,8 +30096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28320,7 +30160,7 @@
       </c>
       <c r="J2" s="22" t="str" cm="1">
         <f t="array" ref="J2">TEXT(_FV(J1,"Price"), IF(_FV(J1,"Price")-_FV(J1,"Previous close",TRUE)&gt;0, "$0.0000▲", "$0.0000▼"))</f>
-        <v>$1.4077▼</v>
+        <v>$1.4075▼</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -37076,8 +38916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38F13E4-FF82-6E40-B343-A0462498EE32}">
   <dimension ref="A1:IT27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added last 12 months chart for BLD
</commit_message>
<xml_diff>
--- a/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
+++ b/Excel Projects/Personal Stock Portfolio/Stock Portfolio Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Personal Stock Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948D0F8F-7549-3040-9E41-2999B0AFDC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41457A55-CCD0-5D47-B625-85E204D31FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -17868,6 +17868,1026 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Close</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1200">
+                <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Last 12 Months </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>BLD!$C$4:$IT$4</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="252"/>
+                <c:pt idx="0">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.63</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.63</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.62</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.44</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.26</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.52</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.43</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.44</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.48</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.52</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.32</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.28</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.28</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.28</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.72</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2.72</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3.04</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2.72</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2.62</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.04</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>3.04</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>3.34</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>3.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-45ED-8E47-BE2E-E669B1CFA305}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1525441008"/>
+        <c:axId val="1525154992"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1525441008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1525154992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1525154992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-C09]* #,##0.00_);_([$$-C09]* \(#,##0.00\);_([$$-C09]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BD"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1525441008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -17986,6 +19006,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -20097,6 +21157,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -20244,6 +21825,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38253</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>45902</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{625DCE63-BFD3-B244-9580-05C4FEC156F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -30096,8 +31715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B311884F-50B8-9E4B-99D7-12BC3BF388CB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38917,7 +40536,7 @@
   <dimension ref="A1:IT27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>